<commit_message>
worked on experimental child psych
</commit_message>
<xml_diff>
--- a/2017 processed/outliers_2017_ari.xlsx
+++ b/2017 processed/outliers_2017_ari.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="10965" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="10965" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CLINICAL" sheetId="1" r:id="rId1"/>
@@ -17,18 +17,14 @@
     <sheet name="SOCIAL" sheetId="3" r:id="rId3"/>
     <sheet name="SPORTS" sheetId="4" r:id="rId4"/>
     <sheet name="IO" sheetId="5" r:id="rId5"/>
+    <sheet name="DEVELOPMENTAL" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4490" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4826" uniqueCount="1074">
   <si>
     <t>Type</t>
   </si>
@@ -3082,6 +3078,174 @@
   </si>
   <si>
     <t>CFA, chi square, parceling approach, mediation model, ANOVA</t>
+  </si>
+  <si>
+    <t>Developmental</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Child Psychology</t>
+  </si>
+  <si>
+    <t>Examining co-occurring and pure relational and physical victimization in early childhood</t>
+  </si>
+  <si>
+    <t>Blakely-McClure, Sarah; Ostrov, Jamie</t>
+  </si>
+  <si>
+    <t>SEM, regression, bifactor model, CFA, chi square</t>
+  </si>
+  <si>
+    <t>The role of declarative and procedural metamemory in event-based prospective memory in school-aged children</t>
+  </si>
+  <si>
+    <t>Cottini, Milvia; et al</t>
+  </si>
+  <si>
+    <t>regression, mixed-effects regression models, ANOVA</t>
+  </si>
+  <si>
+    <t>failed to remember instructions</t>
+  </si>
+  <si>
+    <t>When do you know what you know? The emergence of memory monitoring</t>
+  </si>
+  <si>
+    <t>Liu, Yan; et al</t>
+  </si>
+  <si>
+    <t>answered every question incorrectly, chose same answer for all trials regardless of recognition</t>
+  </si>
+  <si>
+    <t>t-tests, ANOVA, phi correlation</t>
+  </si>
+  <si>
+    <t>lack of attention</t>
+  </si>
+  <si>
+    <t>Observation of directional storybook reading influences young children’s counting direction</t>
+  </si>
+  <si>
+    <t>Gobel, Silke; et al</t>
+  </si>
+  <si>
+    <t>89 books</t>
+  </si>
+  <si>
+    <t>chi square, McNemar's test</t>
+  </si>
+  <si>
+    <t>Using language to get ready: Familiar labels help children to engage proactive control</t>
+  </si>
+  <si>
+    <t>Doebel, Sabine; et al</t>
+  </si>
+  <si>
+    <t>uncooperativeness, experimenter error</t>
+  </si>
+  <si>
+    <t>regression, chi square, maximum-likelihood estimation, log likelihood tests</t>
+  </si>
+  <si>
+    <t>Working memory predicts children’s analogical reasoning</t>
+  </si>
+  <si>
+    <t>Simms, Nina; et al</t>
+  </si>
+  <si>
+    <t>scored excessively low (3 SD)</t>
+  </si>
+  <si>
+    <t>ANOVA, t-tests, regression</t>
+  </si>
+  <si>
+    <t>Intergenerational associations in executive function between mothers and childrenin the context of risk</t>
+  </si>
+  <si>
+    <t>Kim, Matthew; et al</t>
+  </si>
+  <si>
+    <t>OLS regression, t-tests</t>
+  </si>
+  <si>
+    <t>The relationship between executive functioning and language: Examining vocabulary, syntax, and language learning in preschoolers attending HeadStart</t>
+  </si>
+  <si>
+    <t>White, Lisa; et al</t>
+  </si>
+  <si>
+    <t>they checked but found none</t>
+  </si>
+  <si>
+    <t>structural equation modeling, CFA</t>
+  </si>
+  <si>
+    <t>Developmental changes in feature detection across time: Evidence from the attentional blink</t>
+  </si>
+  <si>
+    <t>Russo, Natalie; et al</t>
+  </si>
+  <si>
+    <t>Bonferroni corrections, t-tests, ANOVA</t>
+  </si>
+  <si>
+    <t>‘‘I know something you don’t know”: Discourse and social context effects on the N400 in adolescents</t>
+  </si>
+  <si>
+    <t>Westley, Alexandra; et al</t>
+  </si>
+  <si>
+    <t>technical error, excessive noise in EEG signal, poor comprehension of task</t>
+  </si>
+  <si>
+    <t>Children’s agenda-based regulation: The effects of prior performance and reward on elementary school children’s study choices</t>
+  </si>
+  <si>
+    <t>Lipowski, Stacy; et al</t>
+  </si>
+  <si>
+    <t>The unique and shared contributions of arithmetic operation understanding and numerical magnitude representation to children’s mathematics achievement</t>
+  </si>
+  <si>
+    <t>Wong, Terry Tin-Yau</t>
+  </si>
+  <si>
+    <t>replaced them with values at 3 SD above/below</t>
+  </si>
+  <si>
+    <t>&gt;3 SD above/below the mean</t>
+  </si>
+  <si>
+    <t>chi square, CFA, Akaike information criterion, Bayesian information criterion, regression</t>
+  </si>
+  <si>
+    <t>Input matters: Speed of word recognition in 2-year-olds exposed to multiple accents</t>
+  </si>
+  <si>
+    <t>Buckler, Helen; et al</t>
+  </si>
+  <si>
+    <t>stopped paying attention on later trials; only kept trials with RT 300-2300 ms</t>
+  </si>
+  <si>
+    <t>fussiness during experiment, experimenter error, parental interference, speech delay</t>
+  </si>
+  <si>
+    <t>Improvements in reading accuracy as a result of increased interletter spacing are not specific to children with dyslexia</t>
+  </si>
+  <si>
+    <t>Hakvoort, Britt; et al</t>
+  </si>
+  <si>
+    <t>&gt;3 SD above/below the mean or RT &lt; 200 ms</t>
+  </si>
+  <si>
+    <t>Is processing of symbols and words influenced by writing system? Evidence from Chinese, Korean, English, and Greek</t>
+  </si>
+  <si>
+    <t>technical problems, discrete naming accuracy &lt;67% based on Q-Q plots</t>
+  </si>
+  <si>
+    <t>multigroup path analyses, saturated baseline model, Bayesian information criterion, chi square</t>
   </si>
 </sst>
 </file>
@@ -3156,7 +3320,58 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="86">
+  <dxfs count="103">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -3457,24 +3672,24 @@
     <tableColumn id="13" name="howmanyafterdeletingoutliers"/>
     <tableColumn id="14" name="iftheydidwhatwasthediff"/>
     <tableColumn id="15" name="whatdidtheyfinallyreportgiveresultsover"/>
-    <tableColumn id="16" name="journal_topic (ignore this and on)" dataDxfId="85"/>
-    <tableColumn id="17" name="journal_name" dataDxfId="84"/>
-    <tableColumn id="18" name="year" dataDxfId="83"/>
+    <tableColumn id="16" name="journal_topic (ignore this and on)" dataDxfId="102"/>
+    <tableColumn id="17" name="journal_name" dataDxfId="101"/>
+    <tableColumn id="18" name="year" dataDxfId="100"/>
     <tableColumn id="19" name="participants"/>
-    <tableColumn id="20" name="Basics" dataDxfId="82"/>
-    <tableColumn id="21" name="ANOVA" dataDxfId="81"/>
-    <tableColumn id="22" name="Regression" dataDxfId="80"/>
-    <tableColumn id="23" name="ChiSquare" dataDxfId="79"/>
-    <tableColumn id="24" name="Nonparametric" dataDxfId="78"/>
-    <tableColumn id="25" name="Modeling" dataDxfId="77"/>
-    <tableColumn id="26" name="BayesOther" dataDxfId="76"/>
-    <tableColumn id="27" name="whichexperimentwithinapaper" dataDxfId="75"/>
-    <tableColumn id="28" name="no_participants" dataDxfId="74"/>
-    <tableColumn id="29" name="outliers_yn" dataDxfId="73"/>
-    <tableColumn id="30" name="people_data" dataDxfId="72"/>
-    <tableColumn id="31" name="take_out" dataDxfId="71"/>
-    <tableColumn id="32" name="reasoning_code" dataDxfId="70"/>
-    <tableColumn id="33" name="running_with_out" dataDxfId="69"/>
+    <tableColumn id="20" name="Basics" dataDxfId="99"/>
+    <tableColumn id="21" name="ANOVA" dataDxfId="98"/>
+    <tableColumn id="22" name="Regression" dataDxfId="97"/>
+    <tableColumn id="23" name="ChiSquare" dataDxfId="96"/>
+    <tableColumn id="24" name="Nonparametric" dataDxfId="95"/>
+    <tableColumn id="25" name="Modeling" dataDxfId="94"/>
+    <tableColumn id="26" name="BayesOther" dataDxfId="93"/>
+    <tableColumn id="27" name="whichexperimentwithinapaper" dataDxfId="92"/>
+    <tableColumn id="28" name="no_participants" dataDxfId="91"/>
+    <tableColumn id="29" name="outliers_yn" dataDxfId="90"/>
+    <tableColumn id="30" name="people_data" dataDxfId="89"/>
+    <tableColumn id="31" name="take_out" dataDxfId="88"/>
+    <tableColumn id="32" name="reasoning_code" dataDxfId="87"/>
+    <tableColumn id="33" name="running_with_out" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3499,24 +3714,24 @@
     <tableColumn id="13" name="howmanyafterdeletingoutliers"/>
     <tableColumn id="14" name="iftheydidwhatwasthediff"/>
     <tableColumn id="15" name="whatdidtheyfinallyreportgiveresultsover"/>
-    <tableColumn id="16" name="journal_topic (ignore this and on)" dataDxfId="68"/>
-    <tableColumn id="17" name="journal_name" dataDxfId="67"/>
-    <tableColumn id="18" name="year" dataDxfId="66"/>
+    <tableColumn id="16" name="journal_topic (ignore this and on)" dataDxfId="85"/>
+    <tableColumn id="17" name="journal_name" dataDxfId="84"/>
+    <tableColumn id="18" name="year" dataDxfId="83"/>
     <tableColumn id="19" name="participants"/>
-    <tableColumn id="20" name="Basics" dataDxfId="65"/>
-    <tableColumn id="21" name="ANOVA" dataDxfId="64"/>
-    <tableColumn id="22" name="Regression" dataDxfId="63"/>
-    <tableColumn id="23" name="ChiSquare" dataDxfId="62"/>
-    <tableColumn id="24" name="Nonparametric" dataDxfId="61"/>
-    <tableColumn id="25" name="Modeling" dataDxfId="60"/>
-    <tableColumn id="26" name="BayesOther" dataDxfId="59"/>
-    <tableColumn id="27" name="whichexperimentwithinapaper" dataDxfId="58"/>
-    <tableColumn id="28" name="no_participants" dataDxfId="57"/>
-    <tableColumn id="29" name="outliers_yn" dataDxfId="56"/>
-    <tableColumn id="30" name="people_data" dataDxfId="55"/>
-    <tableColumn id="31" name="take_out" dataDxfId="54"/>
-    <tableColumn id="32" name="reasoning_code" dataDxfId="53"/>
-    <tableColumn id="33" name="running_with_out" dataDxfId="52"/>
+    <tableColumn id="20" name="Basics" dataDxfId="82"/>
+    <tableColumn id="21" name="ANOVA" dataDxfId="81"/>
+    <tableColumn id="22" name="Regression" dataDxfId="80"/>
+    <tableColumn id="23" name="ChiSquare" dataDxfId="79"/>
+    <tableColumn id="24" name="Nonparametric" dataDxfId="78"/>
+    <tableColumn id="25" name="Modeling" dataDxfId="77"/>
+    <tableColumn id="26" name="BayesOther" dataDxfId="76"/>
+    <tableColumn id="27" name="whichexperimentwithinapaper" dataDxfId="75"/>
+    <tableColumn id="28" name="no_participants" dataDxfId="74"/>
+    <tableColumn id="29" name="outliers_yn" dataDxfId="73"/>
+    <tableColumn id="30" name="people_data" dataDxfId="72"/>
+    <tableColumn id="31" name="take_out" dataDxfId="71"/>
+    <tableColumn id="32" name="reasoning_code" dataDxfId="70"/>
+    <tableColumn id="33" name="running_with_out" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3536,7 +3751,49 @@
     <tableColumn id="8" name="wholepeopleorjustdatapoints"/>
     <tableColumn id="9" name="Ifsodidtheytakethemoutorleavethemin"/>
     <tableColumn id="10" name="with, without, or both sets of data ran"/>
-    <tableColumn id="11" name="didtheydescribewhytheytookpploutorlefttheminorciteanyoneforwhyth" dataDxfId="51"/>
+    <tableColumn id="11" name="didtheydescribewhytheytookpploutorlefttheminorciteanyoneforwhyth" dataDxfId="68"/>
+    <tableColumn id="12" name="reasoncoding (leave blank)"/>
+    <tableColumn id="13" name="howmanyafterdeletingoutliers"/>
+    <tableColumn id="14" name="iftheydidwhatwasthediff"/>
+    <tableColumn id="15" name="whatdidtheyfinallyreportgiveresultsover"/>
+    <tableColumn id="16" name="journal_topic (ignore this and on)" dataDxfId="67"/>
+    <tableColumn id="17" name="journal_name" dataDxfId="66"/>
+    <tableColumn id="18" name="year" dataDxfId="65"/>
+    <tableColumn id="19" name="participants"/>
+    <tableColumn id="20" name="Basics" dataDxfId="64"/>
+    <tableColumn id="21" name="ANOVA" dataDxfId="63"/>
+    <tableColumn id="22" name="Regression" dataDxfId="62"/>
+    <tableColumn id="23" name="ChiSquare" dataDxfId="61"/>
+    <tableColumn id="24" name="Nonparametric" dataDxfId="60"/>
+    <tableColumn id="25" name="Modeling" dataDxfId="59"/>
+    <tableColumn id="26" name="BayesOther" dataDxfId="58"/>
+    <tableColumn id="27" name="whichexperimentwithinapaper" dataDxfId="57"/>
+    <tableColumn id="28" name="no_participants" dataDxfId="56"/>
+    <tableColumn id="29" name="outliers_yn" dataDxfId="55"/>
+    <tableColumn id="30" name="people_data" dataDxfId="54"/>
+    <tableColumn id="31" name="take_out" dataDxfId="53"/>
+    <tableColumn id="32" name="reasoning_code" dataDxfId="52"/>
+    <tableColumn id="33" name="running_with_out" dataDxfId="51"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:AG58" totalsRowShown="0">
+  <autoFilter ref="A1:AG58"/>
+  <tableColumns count="33">
+    <tableColumn id="1" name="Type"/>
+    <tableColumn id="2" name="Journal"/>
+    <tableColumn id="3" name="article"/>
+    <tableColumn id="4" name="authors"/>
+    <tableColumn id="5" name="typeofanalysis"/>
+    <tableColumn id="6" name="howmanypplinstudyoriginally"/>
+    <tableColumn id="7" name="dotheymentionoutliers"/>
+    <tableColumn id="8" name="wholepeopleorjustdatapoints"/>
+    <tableColumn id="9" name="Ifsodidtheytakethemoutorleavethemin"/>
+    <tableColumn id="10" name="with, without, or both sets of data ran"/>
+    <tableColumn id="11" name="didtheydescribewhytheytookpploutorlefttheminorciteanyoneforwhyth"/>
     <tableColumn id="12" name="reasoncoding (leave blank)"/>
     <tableColumn id="13" name="howmanyafterdeletingoutliers"/>
     <tableColumn id="14" name="iftheydidwhatwasthediff"/>
@@ -3564,9 +3821,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A1:AG58" totalsRowShown="0">
-  <autoFilter ref="A1:AG58"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:AG125" totalsRowShown="0">
+  <autoFilter ref="A1:AG125"/>
   <tableColumns count="33">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="Journal"/>
@@ -3606,8 +3863,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table156" displayName="Table156" ref="A1:AG125" totalsRowShown="0">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1567" displayName="Table1567" ref="A1:AG125" totalsRowShown="0">
   <autoFilter ref="A1:AG125"/>
   <tableColumns count="33">
     <tableColumn id="1" name="Type"/>
@@ -45406,8 +45663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView topLeftCell="L94" workbookViewId="0">
+      <selection sqref="A1:AG125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50935,4 +51192,3508 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG125"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="F2">
+        <v>231</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F3" s="5">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5">
+        <v>57</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F4" s="5">
+        <v>62</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="M4">
+        <v>58</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1031</v>
+      </c>
+      <c r="M5">
+        <v>63</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F7">
+        <v>147</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="9"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F8">
+        <v>87</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F9">
+        <v>171</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="F10">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M10">
+        <v>64</v>
+      </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1043</v>
+      </c>
+      <c r="F11">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1042</v>
+      </c>
+      <c r="M11">
+        <v>64</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F12">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1050</v>
+      </c>
+      <c r="F13">
+        <v>182</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1049</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F14">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E15" t="s">
+        <v>293</v>
+      </c>
+      <c r="F15">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1056</v>
+      </c>
+      <c r="M15">
+        <v>16</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E16" t="s">
+        <v>430</v>
+      </c>
+      <c r="F16">
+        <f>19+22</f>
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E17" t="s">
+        <v>430</v>
+      </c>
+      <c r="F17">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F18">
+        <v>124</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>170</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1062</v>
+      </c>
+      <c r="M18">
+        <v>124</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E19" t="s">
+        <v>346</v>
+      </c>
+      <c r="F19">
+        <v>32</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" t="s">
+        <v>1066</v>
+      </c>
+      <c r="M19">
+        <v>32</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E20" t="s">
+        <v>346</v>
+      </c>
+      <c r="F20">
+        <v>39</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" t="s">
+        <v>1067</v>
+      </c>
+      <c r="M20">
+        <v>32</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E21" t="s">
+        <v>430</v>
+      </c>
+      <c r="F21">
+        <v>60</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" t="s">
+        <v>170</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1070</v>
+      </c>
+      <c r="M21">
+        <v>60</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E22" t="s">
+        <v>430</v>
+      </c>
+      <c r="F22">
+        <v>189</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" t="s">
+        <v>170</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1070</v>
+      </c>
+      <c r="M22">
+        <v>189</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1073</v>
+      </c>
+      <c r="F23">
+        <f>113+112+100+108</f>
+        <v>433</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" t="s">
+        <v>170</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1072</v>
+      </c>
+      <c r="M23">
+        <v>433</v>
+      </c>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+      <c r="AG30" s="1"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+      <c r="AG31" s="1"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+      <c r="AG33" s="1"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
+      <c r="AG34" s="1"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="1"/>
+      <c r="AG35" s="1"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
+      <c r="AG36" s="1"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
+      <c r="AG37" s="1"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
+      <c r="AG38" s="1"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="1"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
+      <c r="AG39" s="1"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="1"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
+      <c r="AG40" s="1"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="U41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Y41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="1"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
+      <c r="AG41" s="1"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="1"/>
+      <c r="AF42" s="1"/>
+      <c r="AG42" s="1"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Y43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="2"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="U44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="2"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="U45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+      <c r="AG45" s="2"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3"/>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="2"/>
+      <c r="AG46" s="2"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+      <c r="AA47" s="3"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+      <c r="AG47" s="2"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="3"/>
+      <c r="T48" s="3"/>
+      <c r="U48" s="3"/>
+      <c r="V48" s="3"/>
+      <c r="W48" s="3"/>
+      <c r="X48" s="3"/>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="2"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="2"/>
+      <c r="AG48" s="2"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="X49" s="3"/>
+      <c r="Y49" s="3"/>
+      <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="2"/>
+      <c r="AG49" s="2"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+      <c r="AG50" s="2"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="3"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="X51" s="3"/>
+      <c r="Y51" s="3"/>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="2"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="2"/>
+      <c r="AE51" s="2"/>
+      <c r="AF51" s="2"/>
+      <c r="AG51" s="2"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="3"/>
+      <c r="T52" s="3"/>
+      <c r="U52" s="3"/>
+      <c r="V52" s="3"/>
+      <c r="W52" s="3"/>
+      <c r="X52" s="3"/>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2"/>
+      <c r="AE52" s="2"/>
+      <c r="AF52" s="2"/>
+      <c r="AG52" s="2"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="3"/>
+      <c r="T53" s="3"/>
+      <c r="U53" s="3"/>
+      <c r="V53" s="3"/>
+      <c r="W53" s="3"/>
+      <c r="X53" s="3"/>
+      <c r="Y53" s="3"/>
+      <c r="Z53" s="3"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="2"/>
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="2"/>
+      <c r="AE53" s="2"/>
+      <c r="AF53" s="2"/>
+      <c r="AG53" s="2"/>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
+      <c r="X54" s="3"/>
+      <c r="Y54" s="3"/>
+      <c r="Z54" s="3"/>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="2"/>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="2"/>
+      <c r="AE54" s="2"/>
+      <c r="AF54" s="2"/>
+      <c r="AG54" s="2"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="3"/>
+      <c r="T55" s="3"/>
+      <c r="U55" s="3"/>
+      <c r="V55" s="3"/>
+      <c r="W55" s="3"/>
+      <c r="X55" s="3"/>
+      <c r="Y55" s="3"/>
+      <c r="Z55" s="3"/>
+      <c r="AA55" s="3"/>
+      <c r="AB55" s="2"/>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="2"/>
+      <c r="AE55" s="2"/>
+      <c r="AF55" s="2"/>
+      <c r="AG55" s="2"/>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="2"/>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="2"/>
+      <c r="AE56" s="2"/>
+      <c r="AF56" s="2"/>
+      <c r="AG56" s="2"/>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="3"/>
+      <c r="T57" s="3"/>
+      <c r="U57" s="3"/>
+      <c r="V57" s="3"/>
+      <c r="W57" s="3"/>
+      <c r="X57" s="3"/>
+      <c r="Y57" s="3"/>
+      <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="2"/>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="2"/>
+      <c r="AE57" s="2"/>
+      <c r="AF57" s="2"/>
+      <c r="AG57" s="2"/>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
+      <c r="W58" s="3"/>
+      <c r="X58" s="3"/>
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3"/>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="2"/>
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="2"/>
+      <c r="AE58" s="2"/>
+      <c r="AF58" s="2"/>
+      <c r="AG58" s="2"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
+      <c r="W59" s="3"/>
+      <c r="X59" s="3"/>
+      <c r="Y59" s="3"/>
+      <c r="Z59" s="3"/>
+      <c r="AA59" s="3"/>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="2"/>
+      <c r="AE59" s="2"/>
+      <c r="AF59" s="2"/>
+      <c r="AG59" s="2"/>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="3"/>
+      <c r="T60" s="3"/>
+      <c r="U60" s="3"/>
+      <c r="V60" s="3"/>
+      <c r="W60" s="3"/>
+      <c r="X60" s="3"/>
+      <c r="Y60" s="3"/>
+      <c r="Z60" s="3"/>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="2"/>
+      <c r="AC60" s="2"/>
+      <c r="AD60" s="2"/>
+      <c r="AE60" s="2"/>
+      <c r="AF60" s="2"/>
+      <c r="AG60" s="2"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="3"/>
+      <c r="T61" s="3"/>
+      <c r="U61" s="3"/>
+      <c r="V61" s="3"/>
+      <c r="W61" s="3"/>
+      <c r="X61" s="3"/>
+      <c r="Y61" s="3"/>
+      <c r="Z61" s="3"/>
+      <c r="AA61" s="3"/>
+      <c r="AB61" s="2"/>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="2"/>
+      <c r="AE61" s="2"/>
+      <c r="AF61" s="2"/>
+      <c r="AG61" s="2"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+      <c r="X62" s="3"/>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3"/>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="2"/>
+      <c r="AC62" s="2"/>
+      <c r="AD62" s="2"/>
+      <c r="AE62" s="2"/>
+      <c r="AF62" s="2"/>
+      <c r="AG62" s="2"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="3"/>
+      <c r="T63" s="3"/>
+      <c r="U63" s="3"/>
+      <c r="V63" s="3"/>
+      <c r="W63" s="3"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="3"/>
+      <c r="Z63" s="3"/>
+      <c r="AA63" s="3"/>
+      <c r="AB63" s="2"/>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="2"/>
+      <c r="AE63" s="2"/>
+      <c r="AF63" s="2"/>
+      <c r="AG63" s="2"/>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
+      <c r="R64" s="3"/>
+      <c r="T64" s="3"/>
+      <c r="U64" s="3"/>
+      <c r="V64" s="3"/>
+      <c r="W64" s="3"/>
+      <c r="X64" s="3"/>
+      <c r="Y64" s="3"/>
+      <c r="Z64" s="3"/>
+      <c r="AA64" s="3"/>
+      <c r="AB64" s="2"/>
+      <c r="AC64" s="2"/>
+      <c r="AD64" s="2"/>
+      <c r="AE64" s="2"/>
+      <c r="AF64" s="2"/>
+      <c r="AG64" s="2"/>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
+      <c r="R65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="3"/>
+      <c r="V65" s="3"/>
+      <c r="W65" s="3"/>
+      <c r="X65" s="3"/>
+      <c r="Y65" s="3"/>
+      <c r="Z65" s="3"/>
+      <c r="AA65" s="3"/>
+      <c r="AB65" s="2"/>
+      <c r="AC65" s="2"/>
+      <c r="AD65" s="2"/>
+      <c r="AE65" s="2"/>
+      <c r="AF65" s="2"/>
+      <c r="AG65" s="2"/>
+    </row>
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="3"/>
+      <c r="T66" s="3"/>
+      <c r="U66" s="3"/>
+      <c r="V66" s="3"/>
+      <c r="W66" s="3"/>
+      <c r="X66" s="3"/>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3"/>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="2"/>
+      <c r="AC66" s="2"/>
+      <c r="AD66" s="2"/>
+      <c r="AE66" s="2"/>
+      <c r="AF66" s="2"/>
+      <c r="AG66" s="2"/>
+    </row>
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
+      <c r="R67" s="3"/>
+      <c r="T67" s="3"/>
+      <c r="U67" s="3"/>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
+      <c r="X67" s="3"/>
+      <c r="Y67" s="3"/>
+      <c r="Z67" s="3"/>
+      <c r="AA67" s="3"/>
+      <c r="AB67" s="2"/>
+      <c r="AC67" s="2"/>
+      <c r="AD67" s="2"/>
+      <c r="AE67" s="2"/>
+      <c r="AF67" s="2"/>
+      <c r="AG67" s="2"/>
+    </row>
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="3"/>
+      <c r="T68" s="3"/>
+      <c r="U68" s="3"/>
+      <c r="V68" s="3"/>
+      <c r="W68" s="3"/>
+      <c r="X68" s="3"/>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3"/>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="2"/>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="2"/>
+      <c r="AE68" s="2"/>
+      <c r="AF68" s="2"/>
+      <c r="AG68" s="2"/>
+    </row>
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
+      <c r="R69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
+      <c r="V69" s="3"/>
+      <c r="W69" s="3"/>
+      <c r="X69" s="3"/>
+      <c r="Y69" s="3"/>
+      <c r="Z69" s="3"/>
+      <c r="AA69" s="3"/>
+      <c r="AB69" s="2"/>
+      <c r="AC69" s="2"/>
+      <c r="AD69" s="2"/>
+      <c r="AE69" s="2"/>
+      <c r="AF69" s="2"/>
+      <c r="AG69" s="2"/>
+    </row>
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
+      <c r="R70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
+      <c r="X70" s="3"/>
+      <c r="Y70" s="3"/>
+      <c r="Z70" s="3"/>
+      <c r="AA70" s="3"/>
+      <c r="AB70" s="2"/>
+      <c r="AC70" s="2"/>
+      <c r="AD70" s="2"/>
+      <c r="AE70" s="2"/>
+      <c r="AF70" s="2"/>
+      <c r="AG70" s="2"/>
+    </row>
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+      <c r="V71" s="3"/>
+      <c r="W71" s="3"/>
+      <c r="X71" s="3"/>
+      <c r="Y71" s="3"/>
+      <c r="Z71" s="3"/>
+      <c r="AA71" s="3"/>
+      <c r="AB71" s="2"/>
+      <c r="AC71" s="2"/>
+      <c r="AD71" s="2"/>
+      <c r="AE71" s="2"/>
+      <c r="AF71" s="2"/>
+      <c r="AG71" s="2"/>
+    </row>
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="3"/>
+      <c r="T72" s="3"/>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+      <c r="W72" s="3"/>
+      <c r="X72" s="3"/>
+      <c r="Y72" s="3"/>
+      <c r="Z72" s="3"/>
+      <c r="AA72" s="3"/>
+      <c r="AB72" s="2"/>
+      <c r="AC72" s="2"/>
+      <c r="AD72" s="2"/>
+      <c r="AE72" s="2"/>
+      <c r="AF72" s="2"/>
+      <c r="AG72" s="2"/>
+    </row>
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="3"/>
+      <c r="T73" s="3"/>
+      <c r="U73" s="3"/>
+      <c r="V73" s="3"/>
+      <c r="W73" s="3"/>
+      <c r="X73" s="3"/>
+      <c r="Y73" s="3"/>
+      <c r="Z73" s="3"/>
+      <c r="AA73" s="3"/>
+      <c r="AB73" s="2"/>
+      <c r="AC73" s="2"/>
+      <c r="AD73" s="2"/>
+      <c r="AE73" s="2"/>
+      <c r="AF73" s="2"/>
+      <c r="AG73" s="2"/>
+    </row>
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="3"/>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
+      <c r="W74" s="3"/>
+      <c r="X74" s="3"/>
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="3"/>
+      <c r="AA74" s="3"/>
+      <c r="AB74" s="2"/>
+      <c r="AC74" s="2"/>
+      <c r="AD74" s="2"/>
+      <c r="AE74" s="2"/>
+      <c r="AF74" s="2"/>
+      <c r="AG74" s="2"/>
+    </row>
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
+      <c r="V75" s="3"/>
+      <c r="W75" s="3"/>
+      <c r="X75" s="3"/>
+      <c r="Y75" s="3"/>
+      <c r="Z75" s="3"/>
+      <c r="AA75" s="3"/>
+      <c r="AB75" s="2"/>
+      <c r="AC75" s="2"/>
+      <c r="AD75" s="2"/>
+      <c r="AE75" s="2"/>
+      <c r="AF75" s="2"/>
+      <c r="AG75" s="2"/>
+    </row>
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="3"/>
+      <c r="W76" s="3"/>
+      <c r="X76" s="3"/>
+      <c r="Y76" s="3"/>
+      <c r="Z76" s="3"/>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="2"/>
+      <c r="AC76" s="2"/>
+      <c r="AD76" s="2"/>
+      <c r="AE76" s="2"/>
+      <c r="AF76" s="2"/>
+      <c r="AG76" s="2"/>
+    </row>
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="U77" s="3"/>
+      <c r="V77" s="3"/>
+      <c r="W77" s="3"/>
+      <c r="X77" s="3"/>
+      <c r="Y77" s="3"/>
+      <c r="Z77" s="3"/>
+      <c r="AA77" s="3"/>
+      <c r="AB77" s="2"/>
+      <c r="AC77" s="2"/>
+      <c r="AD77" s="2"/>
+      <c r="AE77" s="2"/>
+      <c r="AF77" s="2"/>
+      <c r="AG77" s="2"/>
+    </row>
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3"/>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+      <c r="X78" s="3"/>
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="3"/>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="2"/>
+      <c r="AC78" s="2"/>
+      <c r="AD78" s="2"/>
+      <c r="AE78" s="2"/>
+      <c r="AF78" s="2"/>
+      <c r="AG78" s="2"/>
+    </row>
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+      <c r="R79" s="3"/>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
+      <c r="X79" s="3"/>
+      <c r="Y79" s="3"/>
+      <c r="Z79" s="3"/>
+      <c r="AA79" s="3"/>
+      <c r="AB79" s="2"/>
+      <c r="AC79" s="2"/>
+      <c r="AD79" s="2"/>
+      <c r="AE79" s="2"/>
+      <c r="AF79" s="2"/>
+      <c r="AG79" s="2"/>
+    </row>
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+      <c r="V80" s="3"/>
+      <c r="W80" s="3"/>
+      <c r="X80" s="3"/>
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3"/>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="2"/>
+      <c r="AC80" s="2"/>
+      <c r="AD80" s="2"/>
+      <c r="AE80" s="2"/>
+      <c r="AF80" s="2"/>
+      <c r="AG80" s="2"/>
+    </row>
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="2"/>
+      <c r="R81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
+      <c r="X81" s="3"/>
+      <c r="Y81" s="3"/>
+      <c r="Z81" s="3"/>
+      <c r="AA81" s="3"/>
+      <c r="AB81" s="2"/>
+      <c r="AC81" s="2"/>
+      <c r="AD81" s="2"/>
+      <c r="AE81" s="2"/>
+      <c r="AF81" s="2"/>
+      <c r="AG81" s="2"/>
+    </row>
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3"/>
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+      <c r="X82" s="3"/>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3"/>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="2"/>
+      <c r="AC82" s="2"/>
+      <c r="AD82" s="2"/>
+      <c r="AE82" s="2"/>
+      <c r="AF82" s="2"/>
+      <c r="AG82" s="2"/>
+    </row>
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
+      <c r="X83" s="3"/>
+      <c r="Y83" s="3"/>
+      <c r="Z83" s="3"/>
+      <c r="AA83" s="3"/>
+      <c r="AB83" s="2"/>
+      <c r="AC83" s="2"/>
+      <c r="AD83" s="2"/>
+      <c r="AE83" s="2"/>
+      <c r="AF83" s="2"/>
+      <c r="AG83" s="2"/>
+    </row>
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
+      <c r="R84" s="3"/>
+      <c r="T84" s="3"/>
+      <c r="U84" s="3"/>
+      <c r="V84" s="3"/>
+      <c r="W84" s="3"/>
+      <c r="X84" s="3"/>
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3"/>
+      <c r="AA84" s="3"/>
+      <c r="AB84" s="2"/>
+      <c r="AC84" s="2"/>
+      <c r="AD84" s="2"/>
+      <c r="AE84" s="2"/>
+      <c r="AF84" s="2"/>
+      <c r="AG84" s="2"/>
+    </row>
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
+      <c r="R85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3"/>
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
+      <c r="X85" s="3"/>
+      <c r="Y85" s="3"/>
+      <c r="Z85" s="3"/>
+      <c r="AA85" s="3"/>
+      <c r="AB85" s="2"/>
+      <c r="AC85" s="2"/>
+      <c r="AD85" s="2"/>
+      <c r="AE85" s="2"/>
+      <c r="AF85" s="2"/>
+      <c r="AG85" s="2"/>
+    </row>
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
+      <c r="R86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
+      <c r="X86" s="3"/>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3"/>
+      <c r="AA86" s="3"/>
+      <c r="AB86" s="2"/>
+      <c r="AC86" s="2"/>
+      <c r="AD86" s="2"/>
+      <c r="AE86" s="2"/>
+      <c r="AF86" s="2"/>
+      <c r="AG86" s="2"/>
+    </row>
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="U87" s="3"/>
+      <c r="V87" s="3"/>
+      <c r="W87" s="3"/>
+      <c r="X87" s="3"/>
+      <c r="Y87" s="3"/>
+      <c r="Z87" s="3"/>
+      <c r="AA87" s="3"/>
+      <c r="AB87" s="2"/>
+      <c r="AC87" s="2"/>
+      <c r="AD87" s="2"/>
+      <c r="AE87" s="2"/>
+      <c r="AF87" s="2"/>
+      <c r="AG87" s="2"/>
+    </row>
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P88" s="2"/>
+      <c r="Q88" s="2"/>
+      <c r="R88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="U88" s="3"/>
+      <c r="V88" s="3"/>
+      <c r="W88" s="3"/>
+      <c r="X88" s="3"/>
+      <c r="Y88" s="3"/>
+      <c r="Z88" s="3"/>
+      <c r="AA88" s="3"/>
+      <c r="AB88" s="2"/>
+      <c r="AC88" s="2"/>
+      <c r="AD88" s="2"/>
+      <c r="AE88" s="2"/>
+      <c r="AF88" s="2"/>
+      <c r="AG88" s="2"/>
+    </row>
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P89" s="2"/>
+      <c r="Q89" s="2"/>
+      <c r="R89" s="3"/>
+      <c r="T89" s="3"/>
+      <c r="U89" s="3"/>
+      <c r="V89" s="3"/>
+      <c r="W89" s="3"/>
+      <c r="X89" s="3"/>
+      <c r="Y89" s="3"/>
+      <c r="Z89" s="3"/>
+      <c r="AA89" s="3"/>
+      <c r="AB89" s="2"/>
+      <c r="AC89" s="2"/>
+      <c r="AD89" s="2"/>
+      <c r="AE89" s="2"/>
+      <c r="AF89" s="2"/>
+      <c r="AG89" s="2"/>
+    </row>
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P90" s="2"/>
+      <c r="Q90" s="2"/>
+      <c r="R90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+      <c r="X90" s="3"/>
+      <c r="Y90" s="3"/>
+      <c r="Z90" s="3"/>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="2"/>
+      <c r="AC90" s="2"/>
+      <c r="AD90" s="2"/>
+      <c r="AE90" s="2"/>
+      <c r="AF90" s="2"/>
+      <c r="AG90" s="2"/>
+    </row>
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="2"/>
+      <c r="R91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+      <c r="X91" s="3"/>
+      <c r="Y91" s="3"/>
+      <c r="Z91" s="3"/>
+      <c r="AA91" s="3"/>
+      <c r="AB91" s="2"/>
+      <c r="AC91" s="2"/>
+      <c r="AD91" s="2"/>
+      <c r="AE91" s="2"/>
+      <c r="AF91" s="2"/>
+      <c r="AG91" s="2"/>
+    </row>
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+      <c r="R92" s="3"/>
+      <c r="T92" s="3"/>
+      <c r="U92" s="3"/>
+      <c r="V92" s="3"/>
+      <c r="W92" s="3"/>
+      <c r="X92" s="3"/>
+      <c r="Y92" s="3"/>
+      <c r="Z92" s="3"/>
+      <c r="AA92" s="3"/>
+      <c r="AB92" s="2"/>
+      <c r="AC92" s="2"/>
+      <c r="AD92" s="2"/>
+      <c r="AE92" s="2"/>
+      <c r="AF92" s="2"/>
+      <c r="AG92" s="2"/>
+    </row>
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="3"/>
+      <c r="T93" s="3"/>
+      <c r="U93" s="3"/>
+      <c r="V93" s="3"/>
+      <c r="W93" s="3"/>
+      <c r="X93" s="3"/>
+      <c r="Y93" s="3"/>
+      <c r="Z93" s="3"/>
+      <c r="AA93" s="3"/>
+      <c r="AB93" s="2"/>
+      <c r="AC93" s="2"/>
+      <c r="AD93" s="2"/>
+      <c r="AE93" s="2"/>
+      <c r="AF93" s="2"/>
+      <c r="AG93" s="2"/>
+    </row>
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="2"/>
+      <c r="R94" s="3"/>
+      <c r="T94" s="3"/>
+      <c r="U94" s="3"/>
+      <c r="V94" s="3"/>
+      <c r="W94" s="3"/>
+      <c r="X94" s="3"/>
+      <c r="Y94" s="3"/>
+      <c r="Z94" s="3"/>
+      <c r="AA94" s="3"/>
+      <c r="AB94" s="2"/>
+      <c r="AC94" s="2"/>
+      <c r="AD94" s="2"/>
+      <c r="AE94" s="2"/>
+      <c r="AF94" s="2"/>
+      <c r="AG94" s="2"/>
+    </row>
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="2"/>
+      <c r="R95" s="3"/>
+      <c r="T95" s="3"/>
+      <c r="U95" s="3"/>
+      <c r="V95" s="3"/>
+      <c r="W95" s="3"/>
+      <c r="X95" s="3"/>
+      <c r="Y95" s="3"/>
+      <c r="Z95" s="3"/>
+      <c r="AA95" s="3"/>
+      <c r="AB95" s="2"/>
+      <c r="AC95" s="2"/>
+      <c r="AD95" s="2"/>
+      <c r="AE95" s="2"/>
+      <c r="AF95" s="2"/>
+      <c r="AG95" s="2"/>
+    </row>
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
+      <c r="R96" s="3"/>
+      <c r="T96" s="3"/>
+      <c r="U96" s="3"/>
+      <c r="V96" s="3"/>
+      <c r="W96" s="3"/>
+      <c r="X96" s="3"/>
+      <c r="Y96" s="3"/>
+      <c r="Z96" s="3"/>
+      <c r="AA96" s="3"/>
+      <c r="AB96" s="2"/>
+      <c r="AC96" s="2"/>
+      <c r="AD96" s="2"/>
+      <c r="AE96" s="2"/>
+      <c r="AF96" s="2"/>
+      <c r="AG96" s="2"/>
+    </row>
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P97" s="2"/>
+      <c r="Q97" s="2"/>
+      <c r="R97" s="3"/>
+      <c r="T97" s="3"/>
+      <c r="U97" s="3"/>
+      <c r="V97" s="3"/>
+      <c r="W97" s="3"/>
+      <c r="X97" s="3"/>
+      <c r="Y97" s="3"/>
+      <c r="Z97" s="3"/>
+      <c r="AA97" s="3"/>
+      <c r="AB97" s="2"/>
+      <c r="AC97" s="2"/>
+      <c r="AD97" s="2"/>
+      <c r="AE97" s="2"/>
+      <c r="AF97" s="2"/>
+      <c r="AG97" s="2"/>
+    </row>
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
+      <c r="R98" s="3"/>
+      <c r="T98" s="3"/>
+      <c r="U98" s="3"/>
+      <c r="V98" s="3"/>
+      <c r="W98" s="3"/>
+      <c r="X98" s="3"/>
+      <c r="Y98" s="3"/>
+      <c r="Z98" s="3"/>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="2"/>
+      <c r="AC98" s="2"/>
+      <c r="AD98" s="2"/>
+      <c r="AE98" s="2"/>
+      <c r="AF98" s="2"/>
+      <c r="AG98" s="2"/>
+    </row>
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P99" s="2"/>
+      <c r="Q99" s="2"/>
+      <c r="R99" s="3"/>
+      <c r="T99" s="3"/>
+      <c r="U99" s="3"/>
+      <c r="V99" s="3"/>
+      <c r="W99" s="3"/>
+      <c r="X99" s="3"/>
+      <c r="Y99" s="3"/>
+      <c r="Z99" s="3"/>
+      <c r="AA99" s="3"/>
+      <c r="AB99" s="2"/>
+      <c r="AC99" s="2"/>
+      <c r="AD99" s="2"/>
+      <c r="AE99" s="2"/>
+      <c r="AF99" s="2"/>
+      <c r="AG99" s="2"/>
+    </row>
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P100" s="2"/>
+      <c r="Q100" s="2"/>
+      <c r="R100" s="3"/>
+      <c r="T100" s="3"/>
+      <c r="U100" s="3"/>
+      <c r="V100" s="3"/>
+      <c r="W100" s="3"/>
+      <c r="X100" s="3"/>
+      <c r="Y100" s="3"/>
+      <c r="Z100" s="3"/>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="2"/>
+      <c r="AC100" s="2"/>
+      <c r="AD100" s="2"/>
+      <c r="AE100" s="2"/>
+      <c r="AF100" s="2"/>
+      <c r="AG100" s="2"/>
+    </row>
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
+      <c r="R101" s="3"/>
+      <c r="T101" s="3"/>
+      <c r="U101" s="3"/>
+      <c r="V101" s="3"/>
+      <c r="W101" s="3"/>
+      <c r="X101" s="3"/>
+      <c r="Y101" s="3"/>
+      <c r="Z101" s="3"/>
+      <c r="AA101" s="3"/>
+      <c r="AB101" s="2"/>
+      <c r="AC101" s="2"/>
+      <c r="AD101" s="2"/>
+      <c r="AE101" s="2"/>
+      <c r="AF101" s="2"/>
+      <c r="AG101" s="2"/>
+    </row>
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="3"/>
+      <c r="T102" s="3"/>
+      <c r="U102" s="3"/>
+      <c r="V102" s="3"/>
+      <c r="W102" s="3"/>
+      <c r="X102" s="3"/>
+      <c r="Y102" s="3"/>
+      <c r="Z102" s="3"/>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="2"/>
+      <c r="AC102" s="2"/>
+      <c r="AD102" s="2"/>
+      <c r="AE102" s="2"/>
+      <c r="AF102" s="2"/>
+      <c r="AG102" s="2"/>
+    </row>
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+      <c r="R103" s="3"/>
+      <c r="T103" s="3"/>
+      <c r="U103" s="3"/>
+      <c r="V103" s="3"/>
+      <c r="W103" s="3"/>
+      <c r="X103" s="3"/>
+      <c r="Y103" s="3"/>
+      <c r="Z103" s="3"/>
+      <c r="AA103" s="3"/>
+      <c r="AB103" s="2"/>
+      <c r="AC103" s="2"/>
+      <c r="AD103" s="2"/>
+      <c r="AE103" s="2"/>
+      <c r="AF103" s="2"/>
+      <c r="AG103" s="2"/>
+    </row>
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
+      <c r="R104" s="3"/>
+      <c r="T104" s="3"/>
+      <c r="U104" s="3"/>
+      <c r="V104" s="3"/>
+      <c r="W104" s="3"/>
+      <c r="X104" s="3"/>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="3"/>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="2"/>
+      <c r="AC104" s="2"/>
+      <c r="AD104" s="2"/>
+      <c r="AE104" s="2"/>
+      <c r="AF104" s="2"/>
+      <c r="AG104" s="2"/>
+    </row>
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P105" s="2"/>
+      <c r="Q105" s="2"/>
+      <c r="R105" s="3"/>
+      <c r="T105" s="3"/>
+      <c r="U105" s="3"/>
+      <c r="V105" s="3"/>
+      <c r="W105" s="3"/>
+      <c r="X105" s="3"/>
+      <c r="Y105" s="3"/>
+      <c r="Z105" s="3"/>
+      <c r="AA105" s="3"/>
+      <c r="AB105" s="2"/>
+      <c r="AC105" s="2"/>
+      <c r="AD105" s="2"/>
+      <c r="AE105" s="2"/>
+      <c r="AF105" s="2"/>
+      <c r="AG105" s="2"/>
+    </row>
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P106" s="2"/>
+      <c r="Q106" s="2"/>
+      <c r="R106" s="3"/>
+      <c r="T106" s="3"/>
+      <c r="U106" s="3"/>
+      <c r="V106" s="3"/>
+      <c r="W106" s="3"/>
+      <c r="X106" s="3"/>
+      <c r="Y106" s="3"/>
+      <c r="Z106" s="3"/>
+      <c r="AA106" s="3"/>
+      <c r="AB106" s="2"/>
+      <c r="AC106" s="2"/>
+      <c r="AD106" s="2"/>
+      <c r="AE106" s="2"/>
+      <c r="AF106" s="2"/>
+      <c r="AG106" s="2"/>
+    </row>
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P107" s="2"/>
+      <c r="Q107" s="2"/>
+      <c r="R107" s="3"/>
+      <c r="T107" s="3"/>
+      <c r="U107" s="3"/>
+      <c r="V107" s="3"/>
+      <c r="W107" s="3"/>
+      <c r="X107" s="3"/>
+      <c r="Y107" s="3"/>
+      <c r="Z107" s="3"/>
+      <c r="AA107" s="3"/>
+      <c r="AB107" s="2"/>
+      <c r="AC107" s="2"/>
+      <c r="AD107" s="2"/>
+      <c r="AE107" s="2"/>
+      <c r="AF107" s="2"/>
+      <c r="AG107" s="2"/>
+    </row>
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P108" s="2"/>
+      <c r="Q108" s="2"/>
+      <c r="R108" s="3"/>
+      <c r="T108" s="3"/>
+      <c r="U108" s="3"/>
+      <c r="V108" s="3"/>
+      <c r="W108" s="3"/>
+      <c r="X108" s="3"/>
+      <c r="Y108" s="3"/>
+      <c r="Z108" s="3"/>
+      <c r="AA108" s="3"/>
+      <c r="AB108" s="2"/>
+      <c r="AC108" s="2"/>
+      <c r="AD108" s="2"/>
+      <c r="AE108" s="2"/>
+      <c r="AF108" s="2"/>
+      <c r="AG108" s="2"/>
+    </row>
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="2"/>
+      <c r="R109" s="3"/>
+      <c r="T109" s="3"/>
+      <c r="U109" s="3"/>
+      <c r="V109" s="3"/>
+      <c r="W109" s="3"/>
+      <c r="X109" s="3"/>
+      <c r="Y109" s="3"/>
+      <c r="Z109" s="3"/>
+      <c r="AA109" s="3"/>
+      <c r="AB109" s="2"/>
+      <c r="AC109" s="2"/>
+      <c r="AD109" s="2"/>
+      <c r="AE109" s="2"/>
+      <c r="AF109" s="2"/>
+      <c r="AG109" s="2"/>
+    </row>
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
+      <c r="R110" s="3"/>
+      <c r="T110" s="3"/>
+      <c r="U110" s="3"/>
+      <c r="V110" s="3"/>
+      <c r="W110" s="3"/>
+      <c r="X110" s="3"/>
+      <c r="Y110" s="3"/>
+      <c r="Z110" s="3"/>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="2"/>
+      <c r="AC110" s="2"/>
+      <c r="AD110" s="2"/>
+      <c r="AE110" s="2"/>
+      <c r="AF110" s="2"/>
+      <c r="AG110" s="2"/>
+    </row>
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P111" s="2"/>
+      <c r="Q111" s="2"/>
+      <c r="R111" s="3"/>
+      <c r="T111" s="3"/>
+      <c r="U111" s="3"/>
+      <c r="V111" s="3"/>
+      <c r="W111" s="3"/>
+      <c r="X111" s="3"/>
+      <c r="Y111" s="3"/>
+      <c r="Z111" s="3"/>
+      <c r="AA111" s="3"/>
+      <c r="AB111" s="2"/>
+      <c r="AC111" s="2"/>
+      <c r="AD111" s="2"/>
+      <c r="AE111" s="2"/>
+      <c r="AF111" s="2"/>
+      <c r="AG111" s="2"/>
+    </row>
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
+      <c r="R112" s="3"/>
+      <c r="T112" s="3"/>
+      <c r="U112" s="3"/>
+      <c r="V112" s="3"/>
+      <c r="W112" s="3"/>
+      <c r="X112" s="3"/>
+      <c r="Y112" s="3"/>
+      <c r="Z112" s="3"/>
+      <c r="AA112" s="3"/>
+      <c r="AB112" s="2"/>
+      <c r="AC112" s="2"/>
+      <c r="AD112" s="2"/>
+      <c r="AE112" s="2"/>
+      <c r="AF112" s="2"/>
+      <c r="AG112" s="2"/>
+    </row>
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P113" s="2"/>
+      <c r="Q113" s="2"/>
+      <c r="R113" s="3"/>
+      <c r="T113" s="3"/>
+      <c r="U113" s="3"/>
+      <c r="V113" s="3"/>
+      <c r="W113" s="3"/>
+      <c r="X113" s="3"/>
+      <c r="Y113" s="3"/>
+      <c r="Z113" s="3"/>
+      <c r="AA113" s="3"/>
+      <c r="AB113" s="2"/>
+      <c r="AC113" s="2"/>
+      <c r="AD113" s="2"/>
+      <c r="AE113" s="2"/>
+      <c r="AF113" s="2"/>
+      <c r="AG113" s="2"/>
+    </row>
+    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+      <c r="R114" s="3"/>
+      <c r="T114" s="3"/>
+      <c r="U114" s="3"/>
+      <c r="V114" s="3"/>
+      <c r="W114" s="3"/>
+      <c r="X114" s="3"/>
+      <c r="Y114" s="3"/>
+      <c r="Z114" s="3"/>
+      <c r="AA114" s="3"/>
+      <c r="AB114" s="2"/>
+      <c r="AC114" s="2"/>
+      <c r="AD114" s="2"/>
+      <c r="AE114" s="2"/>
+      <c r="AF114" s="2"/>
+      <c r="AG114" s="2"/>
+    </row>
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="2"/>
+      <c r="R115" s="3"/>
+      <c r="T115" s="3"/>
+      <c r="U115" s="3"/>
+      <c r="V115" s="3"/>
+      <c r="W115" s="3"/>
+      <c r="X115" s="3"/>
+      <c r="Y115" s="3"/>
+      <c r="Z115" s="3"/>
+      <c r="AA115" s="3"/>
+      <c r="AB115" s="2"/>
+      <c r="AC115" s="2"/>
+      <c r="AD115" s="2"/>
+      <c r="AE115" s="2"/>
+      <c r="AF115" s="2"/>
+      <c r="AG115" s="2"/>
+    </row>
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="2"/>
+      <c r="R116" s="3"/>
+      <c r="T116" s="3"/>
+      <c r="U116" s="3"/>
+      <c r="V116" s="3"/>
+      <c r="W116" s="3"/>
+      <c r="X116" s="3"/>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3"/>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="2"/>
+      <c r="AC116" s="2"/>
+      <c r="AD116" s="2"/>
+      <c r="AE116" s="2"/>
+      <c r="AF116" s="2"/>
+      <c r="AG116" s="2"/>
+    </row>
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="3"/>
+      <c r="T117" s="3"/>
+      <c r="U117" s="3"/>
+      <c r="V117" s="3"/>
+      <c r="W117" s="3"/>
+      <c r="X117" s="3"/>
+      <c r="Y117" s="3"/>
+      <c r="Z117" s="3"/>
+      <c r="AA117" s="3"/>
+      <c r="AB117" s="2"/>
+      <c r="AC117" s="2"/>
+      <c r="AD117" s="2"/>
+      <c r="AE117" s="2"/>
+      <c r="AF117" s="2"/>
+      <c r="AG117" s="2"/>
+    </row>
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
+      <c r="R118" s="3"/>
+      <c r="T118" s="3"/>
+      <c r="U118" s="3"/>
+      <c r="V118" s="3"/>
+      <c r="W118" s="3"/>
+      <c r="X118" s="3"/>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3"/>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="2"/>
+      <c r="AC118" s="2"/>
+      <c r="AD118" s="2"/>
+      <c r="AE118" s="2"/>
+      <c r="AF118" s="2"/>
+      <c r="AG118" s="2"/>
+    </row>
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="2"/>
+      <c r="R119" s="3"/>
+      <c r="T119" s="3"/>
+      <c r="U119" s="3"/>
+      <c r="V119" s="3"/>
+      <c r="W119" s="3"/>
+      <c r="X119" s="3"/>
+      <c r="Y119" s="3"/>
+      <c r="Z119" s="3"/>
+      <c r="AA119" s="3"/>
+      <c r="AB119" s="2"/>
+      <c r="AC119" s="2"/>
+      <c r="AD119" s="2"/>
+      <c r="AE119" s="2"/>
+      <c r="AF119" s="2"/>
+      <c r="AG119" s="2"/>
+    </row>
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="2"/>
+      <c r="R120" s="3"/>
+      <c r="T120" s="3"/>
+      <c r="U120" s="3"/>
+      <c r="V120" s="3"/>
+      <c r="W120" s="3"/>
+      <c r="X120" s="3"/>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3"/>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="2"/>
+      <c r="AC120" s="2"/>
+      <c r="AD120" s="2"/>
+      <c r="AE120" s="2"/>
+      <c r="AF120" s="2"/>
+      <c r="AG120" s="2"/>
+    </row>
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P121" s="2"/>
+      <c r="Q121" s="2"/>
+      <c r="R121" s="3"/>
+      <c r="T121" s="3"/>
+      <c r="U121" s="3"/>
+      <c r="V121" s="3"/>
+      <c r="W121" s="3"/>
+      <c r="X121" s="3"/>
+      <c r="Y121" s="3"/>
+      <c r="Z121" s="3"/>
+      <c r="AA121" s="3"/>
+      <c r="AB121" s="2"/>
+      <c r="AC121" s="2"/>
+      <c r="AD121" s="2"/>
+      <c r="AE121" s="2"/>
+      <c r="AF121" s="2"/>
+      <c r="AG121" s="2"/>
+    </row>
+    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P122" s="2"/>
+      <c r="Q122" s="2"/>
+      <c r="R122" s="3"/>
+      <c r="T122" s="3"/>
+      <c r="U122" s="3"/>
+      <c r="V122" s="3"/>
+      <c r="W122" s="3"/>
+      <c r="X122" s="3"/>
+      <c r="Y122" s="3"/>
+      <c r="Z122" s="3"/>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="2"/>
+      <c r="AC122" s="2"/>
+      <c r="AD122" s="2"/>
+      <c r="AE122" s="2"/>
+      <c r="AF122" s="2"/>
+      <c r="AG122" s="2"/>
+    </row>
+    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P123" s="2"/>
+      <c r="Q123" s="2"/>
+      <c r="R123" s="3"/>
+      <c r="T123" s="3"/>
+      <c r="U123" s="3"/>
+      <c r="V123" s="3"/>
+      <c r="W123" s="3"/>
+      <c r="X123" s="3"/>
+      <c r="Y123" s="3"/>
+      <c r="Z123" s="3"/>
+      <c r="AA123" s="3"/>
+      <c r="AB123" s="2"/>
+      <c r="AC123" s="2"/>
+      <c r="AD123" s="2"/>
+      <c r="AE123" s="2"/>
+      <c r="AF123" s="2"/>
+      <c r="AG123" s="2"/>
+    </row>
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P124" s="2"/>
+      <c r="Q124" s="2"/>
+      <c r="R124" s="3"/>
+      <c r="T124" s="3"/>
+      <c r="U124" s="3"/>
+      <c r="V124" s="3"/>
+      <c r="W124" s="3"/>
+      <c r="X124" s="3"/>
+      <c r="Y124" s="3"/>
+      <c r="Z124" s="3"/>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="2"/>
+      <c r="AC124" s="2"/>
+      <c r="AD124" s="2"/>
+      <c r="AE124" s="2"/>
+      <c r="AF124" s="2"/>
+      <c r="AG124" s="2"/>
+    </row>
+    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="3"/>
+      <c r="T125" s="3"/>
+      <c r="U125" s="3"/>
+      <c r="V125" s="3"/>
+      <c r="W125" s="3"/>
+      <c r="X125" s="3"/>
+      <c r="Y125" s="3"/>
+      <c r="Z125" s="3"/>
+      <c r="AA125" s="3"/>
+      <c r="AB125" s="2"/>
+      <c r="AC125" s="2"/>
+      <c r="AD125" s="2"/>
+      <c r="AE125" s="2"/>
+      <c r="AF125" s="2"/>
+      <c r="AG125" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished Experimental Child Psych
</commit_message>
<xml_diff>
--- a/2017 processed/outliers_2017_ari.xlsx
+++ b/2017 processed/outliers_2017_ari.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4826" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4806" uniqueCount="1106">
   <si>
     <t>Type</t>
   </si>
@@ -3246,6 +3246,102 @@
   </si>
   <si>
     <t>multigroup path analyses, saturated baseline model, Bayesian information criterion, chi square</t>
+  </si>
+  <si>
+    <t>Altani, Angeliki; et al</t>
+  </si>
+  <si>
+    <t>Van de Vondervoort, Julia; Hamlin, J. Kiley</t>
+  </si>
+  <si>
+    <t>Preschoolers’ social and moral judgments ofthird-party helpers and hinderers align withinfants’ social evaluations</t>
+  </si>
+  <si>
+    <t>uncooperativeness, interference from parents, procedure errors, failure to complete English comprehension task</t>
+  </si>
+  <si>
+    <t>uncooperativeness</t>
+  </si>
+  <si>
+    <t>Developmental changes in the mental transformation of spatial arrays</t>
+  </si>
+  <si>
+    <t>Michaelides, Christos; Avraamides, Marios</t>
+  </si>
+  <si>
+    <t>ANOVA, correlations</t>
+  </si>
+  <si>
+    <t>Children’s developing metaethical judgments</t>
+  </si>
+  <si>
+    <t>Schmidt, Marco; et al</t>
+  </si>
+  <si>
+    <t>experimenter error, equipment malfunction, uncooperativeness</t>
+  </si>
+  <si>
+    <t>generalized linear mixed models, likelihood ratio test, chi square, Wilcoxon signed-rank tests</t>
+  </si>
+  <si>
+    <t>Bilingual children’s social preferences hinge on accent</t>
+  </si>
+  <si>
+    <t>DeJesus, Jasmine; et al</t>
+  </si>
+  <si>
+    <t>Statistical learning of speech sounds is most robust during the period of perceptual attunement</t>
+  </si>
+  <si>
+    <t>Liu, Liquan; Kager, Rene</t>
+  </si>
+  <si>
+    <t>excessive fussiness, parental interference, "looking time not reaching 60% of the total looking time during the familiarization phase", failure to habituate, looking time less than 2s, statistical outliers in looking time (2+ SD)</t>
+  </si>
+  <si>
+    <t>Characteristics of brief sticky mittens training that lead to increases in object exploration</t>
+  </si>
+  <si>
+    <t>Needham, Amy; et al</t>
+  </si>
+  <si>
+    <t>incomplete video recordings, excessive fussiness, "successful independent reaching in the pretraining session"</t>
+  </si>
+  <si>
+    <t>t-tests, ANCOVA</t>
+  </si>
+  <si>
+    <t>fussiness, experimenter error, "successful independent reaching in the pretraining session"</t>
+  </si>
+  <si>
+    <t>Theory of mind in emerging reading comprehension: A longitudinal study of early indirect and direct effects</t>
+  </si>
+  <si>
+    <t>Atkinson, Lynette; et al</t>
+  </si>
+  <si>
+    <t>Adding sound to theory of mind: Comparing children’s development of mental-state understanding in the auditory and visual realms</t>
+  </si>
+  <si>
+    <t>Hasni, Anita; et al</t>
+  </si>
+  <si>
+    <t>Developmental changes in maternal education and minimal exposure effects on vocabulary in English- and Spanish-learning toddlers</t>
+  </si>
+  <si>
+    <t>Friend, Margaret; et al</t>
+  </si>
+  <si>
+    <t>t-tests, ANCOVA, correlations</t>
+  </si>
+  <si>
+    <t>Getting to the elephants: Gesture and preschoolers’ comprehension of route direction information</t>
+  </si>
+  <si>
+    <t>Austin, Elizabeth; Sweller, Naomi</t>
+  </si>
+  <si>
+    <t>ICC, ANOVA</t>
   </si>
 </sst>
 </file>
@@ -3864,8 +3960,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1567" displayName="Table1567" ref="A1:AG125" totalsRowShown="0">
-  <autoFilter ref="A1:AG125"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1567" displayName="Table1567" ref="A1:AG36" totalsRowShown="0">
+  <autoFilter ref="A1:AG36"/>
   <tableColumns count="33">
     <tableColumn id="1" name="Type"/>
     <tableColumn id="2" name="Journal"/>
@@ -51196,16 +51292,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG125"/>
+  <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.140625" customWidth="1"/>
@@ -52339,6 +52435,9 @@
       <c r="C23" t="s">
         <v>1071</v>
       </c>
+      <c r="D23" t="s">
+        <v>1074</v>
+      </c>
       <c r="E23" t="s">
         <v>1073</v>
       </c>
@@ -52389,6 +52488,36 @@
       <c r="B24" t="s">
         <v>1019</v>
       </c>
+      <c r="C24" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E24" t="s">
+        <v>430</v>
+      </c>
+      <c r="F24">
+        <v>86</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" t="s">
+        <v>1077</v>
+      </c>
+      <c r="M24">
+        <v>74</v>
+      </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="3"/>
@@ -52414,6 +52543,36 @@
       <c r="B25" t="s">
         <v>1019</v>
       </c>
+      <c r="C25" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E25" t="s">
+        <v>430</v>
+      </c>
+      <c r="F25">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1078</v>
+      </c>
+      <c r="M25">
+        <v>24</v>
+      </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="3"/>
@@ -52439,7 +52598,22 @@
       <c r="B26" t="s">
         <v>1019</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="C26" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F26" s="5">
+        <f>39+47+35+30</f>
+        <v>151</v>
+      </c>
+      <c r="G26" t="s">
+        <v>40</v>
+      </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="3"/>
@@ -52465,6 +52639,36 @@
       <c r="B27" t="s">
         <v>1019</v>
       </c>
+      <c r="C27" t="s">
+        <v>1082</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F27">
+        <v>148</v>
+      </c>
+      <c r="G27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s">
+        <v>1084</v>
+      </c>
+      <c r="M27">
+        <v>136</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="3"/>
@@ -52490,6 +52694,21 @@
       <c r="B28" t="s">
         <v>1019</v>
       </c>
+      <c r="C28" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E28" t="s">
+        <v>293</v>
+      </c>
+      <c r="F28">
+        <v>40</v>
+      </c>
+      <c r="G28" t="s">
+        <v>40</v>
+      </c>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="3"/>
@@ -52515,6 +52734,21 @@
       <c r="B29" t="s">
         <v>1019</v>
       </c>
+      <c r="C29" t="s">
+        <v>1086</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E29" t="s">
+        <v>293</v>
+      </c>
+      <c r="F29">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>40</v>
+      </c>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="3"/>
@@ -52540,6 +52774,36 @@
       <c r="B30" t="s">
         <v>1019</v>
       </c>
+      <c r="C30" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E30" t="s">
+        <v>293</v>
+      </c>
+      <c r="F30">
+        <v>134</v>
+      </c>
+      <c r="G30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" t="s">
+        <v>1090</v>
+      </c>
+      <c r="M30">
+        <v>88</v>
+      </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="3"/>
@@ -52565,6 +52829,36 @@
       <c r="B31" t="s">
         <v>1019</v>
       </c>
+      <c r="C31" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1094</v>
+      </c>
+      <c r="F31">
+        <v>45</v>
+      </c>
+      <c r="G31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" t="s">
+        <v>1093</v>
+      </c>
+      <c r="M31">
+        <v>38</v>
+      </c>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="3"/>
@@ -52590,6 +52884,37 @@
       <c r="B32" t="s">
         <v>1019</v>
       </c>
+      <c r="C32" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E32" t="s">
+        <v>430</v>
+      </c>
+      <c r="F32">
+        <f>36+19</f>
+        <v>55</v>
+      </c>
+      <c r="G32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1095</v>
+      </c>
+      <c r="M32">
+        <v>36</v>
+      </c>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="3"/>
@@ -52615,6 +52940,21 @@
       <c r="B33" t="s">
         <v>1019</v>
       </c>
+      <c r="C33" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E33" t="s">
+        <v>853</v>
+      </c>
+      <c r="F33">
+        <v>80</v>
+      </c>
+      <c r="G33" t="s">
+        <v>40</v>
+      </c>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="3"/>
@@ -52640,6 +52980,21 @@
       <c r="B34" t="s">
         <v>1019</v>
       </c>
+      <c r="C34" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34">
+        <v>66</v>
+      </c>
+      <c r="G34" t="s">
+        <v>40</v>
+      </c>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="3"/>
@@ -52665,6 +53020,22 @@
       <c r="B35" t="s">
         <v>1019</v>
       </c>
+      <c r="C35" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F35">
+        <f>71+56+26</f>
+        <v>153</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="3"/>
@@ -52690,6 +53061,21 @@
       <c r="B36" t="s">
         <v>1019</v>
       </c>
+      <c r="C36" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F36">
+        <v>174</v>
+      </c>
+      <c r="G36" t="s">
+        <v>40</v>
+      </c>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="3"/>
@@ -52708,1988 +53094,6 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="W37" s="3"/>
-      <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-      <c r="Z37" s="3"/>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="2"/>
-      <c r="AC37" s="2"/>
-      <c r="AD37" s="1"/>
-      <c r="AE37" s="1"/>
-      <c r="AF37" s="1"/>
-      <c r="AG37" s="1"/>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AA38" s="3"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="2"/>
-      <c r="AD38" s="1"/>
-      <c r="AE38" s="1"/>
-      <c r="AF38" s="1"/>
-      <c r="AG38" s="1"/>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AA39" s="3"/>
-      <c r="AB39" s="2"/>
-      <c r="AC39" s="2"/>
-      <c r="AD39" s="1"/>
-      <c r="AE39" s="1"/>
-      <c r="AF39" s="1"/>
-      <c r="AG39" s="1"/>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AA40" s="3"/>
-      <c r="AB40" s="2"/>
-      <c r="AC40" s="2"/>
-      <c r="AD40" s="1"/>
-      <c r="AE40" s="1"/>
-      <c r="AF40" s="1"/>
-      <c r="AG40" s="1"/>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AA41" s="3"/>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="1"/>
-      <c r="AE41" s="1"/>
-      <c r="AF41" s="1"/>
-      <c r="AG41" s="1"/>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="2"/>
-      <c r="AC42" s="2"/>
-      <c r="AD42" s="1"/>
-      <c r="AE42" s="1"/>
-      <c r="AF42" s="1"/>
-      <c r="AG42" s="1"/>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AA43" s="3"/>
-      <c r="AB43" s="2"/>
-      <c r="AC43" s="2"/>
-      <c r="AD43" s="2"/>
-      <c r="AE43" s="2"/>
-      <c r="AF43" s="2"/>
-      <c r="AG43" s="2"/>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1019</v>
-      </c>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="2"/>
-      <c r="AC44" s="2"/>
-      <c r="AD44" s="2"/>
-      <c r="AE44" s="2"/>
-      <c r="AF44" s="2"/>
-      <c r="AG44" s="2"/>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
-      <c r="AA45" s="3"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="2"/>
-      <c r="AD45" s="2"/>
-      <c r="AE45" s="2"/>
-      <c r="AF45" s="2"/>
-      <c r="AG45" s="2"/>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="2"/>
-      <c r="AC46" s="2"/>
-      <c r="AD46" s="2"/>
-      <c r="AE46" s="2"/>
-      <c r="AF46" s="2"/>
-      <c r="AG46" s="2"/>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-      <c r="AA47" s="3"/>
-      <c r="AB47" s="2"/>
-      <c r="AC47" s="2"/>
-      <c r="AD47" s="2"/>
-      <c r="AE47" s="2"/>
-      <c r="AF47" s="2"/>
-      <c r="AG47" s="2"/>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-      <c r="AA48" s="3"/>
-      <c r="AB48" s="2"/>
-      <c r="AC48" s="2"/>
-      <c r="AD48" s="2"/>
-      <c r="AE48" s="2"/>
-      <c r="AF48" s="2"/>
-      <c r="AG48" s="2"/>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
-      <c r="X49" s="3"/>
-      <c r="Y49" s="3"/>
-      <c r="Z49" s="3"/>
-      <c r="AA49" s="3"/>
-      <c r="AB49" s="2"/>
-      <c r="AC49" s="2"/>
-      <c r="AD49" s="2"/>
-      <c r="AE49" s="2"/>
-      <c r="AF49" s="2"/>
-      <c r="AG49" s="2"/>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
-      <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-      <c r="AA50" s="3"/>
-      <c r="AB50" s="2"/>
-      <c r="AC50" s="2"/>
-      <c r="AD50" s="2"/>
-      <c r="AE50" s="2"/>
-      <c r="AF50" s="2"/>
-      <c r="AG50" s="2"/>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-      <c r="AA51" s="3"/>
-      <c r="AB51" s="2"/>
-      <c r="AC51" s="2"/>
-      <c r="AD51" s="2"/>
-      <c r="AE51" s="2"/>
-      <c r="AF51" s="2"/>
-      <c r="AG51" s="2"/>
-    </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
-      <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
-      <c r="Z52" s="3"/>
-      <c r="AA52" s="3"/>
-      <c r="AB52" s="2"/>
-      <c r="AC52" s="2"/>
-      <c r="AD52" s="2"/>
-      <c r="AE52" s="2"/>
-      <c r="AF52" s="2"/>
-      <c r="AG52" s="2"/>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="3"/>
-      <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-      <c r="V53" s="3"/>
-      <c r="W53" s="3"/>
-      <c r="X53" s="3"/>
-      <c r="Y53" s="3"/>
-      <c r="Z53" s="3"/>
-      <c r="AA53" s="3"/>
-      <c r="AB53" s="2"/>
-      <c r="AC53" s="2"/>
-      <c r="AD53" s="2"/>
-      <c r="AE53" s="2"/>
-      <c r="AF53" s="2"/>
-      <c r="AG53" s="2"/>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="3"/>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-      <c r="V54" s="3"/>
-      <c r="W54" s="3"/>
-      <c r="X54" s="3"/>
-      <c r="Y54" s="3"/>
-      <c r="Z54" s="3"/>
-      <c r="AA54" s="3"/>
-      <c r="AB54" s="2"/>
-      <c r="AC54" s="2"/>
-      <c r="AD54" s="2"/>
-      <c r="AE54" s="2"/>
-      <c r="AF54" s="2"/>
-      <c r="AG54" s="2"/>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P55" s="2"/>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
-      <c r="Z55" s="3"/>
-      <c r="AA55" s="3"/>
-      <c r="AB55" s="2"/>
-      <c r="AC55" s="2"/>
-      <c r="AD55" s="2"/>
-      <c r="AE55" s="2"/>
-      <c r="AF55" s="2"/>
-      <c r="AG55" s="2"/>
-    </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="3"/>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
-      <c r="V56" s="3"/>
-      <c r="W56" s="3"/>
-      <c r="X56" s="3"/>
-      <c r="Y56" s="3"/>
-      <c r="Z56" s="3"/>
-      <c r="AA56" s="3"/>
-      <c r="AB56" s="2"/>
-      <c r="AC56" s="2"/>
-      <c r="AD56" s="2"/>
-      <c r="AE56" s="2"/>
-      <c r="AF56" s="2"/>
-      <c r="AG56" s="2"/>
-    </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
-      <c r="X57" s="3"/>
-      <c r="Y57" s="3"/>
-      <c r="Z57" s="3"/>
-      <c r="AA57" s="3"/>
-      <c r="AB57" s="2"/>
-      <c r="AC57" s="2"/>
-      <c r="AD57" s="2"/>
-      <c r="AE57" s="2"/>
-      <c r="AF57" s="2"/>
-      <c r="AG57" s="2"/>
-    </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
-      <c r="Z58" s="3"/>
-      <c r="AA58" s="3"/>
-      <c r="AB58" s="2"/>
-      <c r="AC58" s="2"/>
-      <c r="AD58" s="2"/>
-      <c r="AE58" s="2"/>
-      <c r="AF58" s="2"/>
-      <c r="AG58" s="2"/>
-    </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
-      <c r="W59" s="3"/>
-      <c r="X59" s="3"/>
-      <c r="Y59" s="3"/>
-      <c r="Z59" s="3"/>
-      <c r="AA59" s="3"/>
-      <c r="AB59" s="2"/>
-      <c r="AC59" s="2"/>
-      <c r="AD59" s="2"/>
-      <c r="AE59" s="2"/>
-      <c r="AF59" s="2"/>
-      <c r="AG59" s="2"/>
-    </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
-      <c r="X60" s="3"/>
-      <c r="Y60" s="3"/>
-      <c r="Z60" s="3"/>
-      <c r="AA60" s="3"/>
-      <c r="AB60" s="2"/>
-      <c r="AC60" s="2"/>
-      <c r="AD60" s="2"/>
-      <c r="AE60" s="2"/>
-      <c r="AF60" s="2"/>
-      <c r="AG60" s="2"/>
-    </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2"/>
-      <c r="R61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
-      <c r="X61" s="3"/>
-      <c r="Y61" s="3"/>
-      <c r="Z61" s="3"/>
-      <c r="AA61" s="3"/>
-      <c r="AB61" s="2"/>
-      <c r="AC61" s="2"/>
-      <c r="AD61" s="2"/>
-      <c r="AE61" s="2"/>
-      <c r="AF61" s="2"/>
-      <c r="AG61" s="2"/>
-    </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
-      <c r="W62" s="3"/>
-      <c r="X62" s="3"/>
-      <c r="Y62" s="3"/>
-      <c r="Z62" s="3"/>
-      <c r="AA62" s="3"/>
-      <c r="AB62" s="2"/>
-      <c r="AC62" s="2"/>
-      <c r="AD62" s="2"/>
-      <c r="AE62" s="2"/>
-      <c r="AF62" s="2"/>
-      <c r="AG62" s="2"/>
-    </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="R63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-      <c r="V63" s="3"/>
-      <c r="W63" s="3"/>
-      <c r="X63" s="3"/>
-      <c r="Y63" s="3"/>
-      <c r="Z63" s="3"/>
-      <c r="AA63" s="3"/>
-      <c r="AB63" s="2"/>
-      <c r="AC63" s="2"/>
-      <c r="AD63" s="2"/>
-      <c r="AE63" s="2"/>
-      <c r="AF63" s="2"/>
-      <c r="AG63" s="2"/>
-    </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-      <c r="R64" s="3"/>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
-      <c r="V64" s="3"/>
-      <c r="W64" s="3"/>
-      <c r="X64" s="3"/>
-      <c r="Y64" s="3"/>
-      <c r="Z64" s="3"/>
-      <c r="AA64" s="3"/>
-      <c r="AB64" s="2"/>
-      <c r="AC64" s="2"/>
-      <c r="AD64" s="2"/>
-      <c r="AE64" s="2"/>
-      <c r="AF64" s="2"/>
-      <c r="AG64" s="2"/>
-    </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P65" s="2"/>
-      <c r="Q65" s="2"/>
-      <c r="R65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
-      <c r="X65" s="3"/>
-      <c r="Y65" s="3"/>
-      <c r="Z65" s="3"/>
-      <c r="AA65" s="3"/>
-      <c r="AB65" s="2"/>
-      <c r="AC65" s="2"/>
-      <c r="AD65" s="2"/>
-      <c r="AE65" s="2"/>
-      <c r="AF65" s="2"/>
-      <c r="AG65" s="2"/>
-    </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="3"/>
-      <c r="T66" s="3"/>
-      <c r="U66" s="3"/>
-      <c r="V66" s="3"/>
-      <c r="W66" s="3"/>
-      <c r="X66" s="3"/>
-      <c r="Y66" s="3"/>
-      <c r="Z66" s="3"/>
-      <c r="AA66" s="3"/>
-      <c r="AB66" s="2"/>
-      <c r="AC66" s="2"/>
-      <c r="AD66" s="2"/>
-      <c r="AE66" s="2"/>
-      <c r="AF66" s="2"/>
-      <c r="AG66" s="2"/>
-    </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
-      <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
-      <c r="X67" s="3"/>
-      <c r="Y67" s="3"/>
-      <c r="Z67" s="3"/>
-      <c r="AA67" s="3"/>
-      <c r="AB67" s="2"/>
-      <c r="AC67" s="2"/>
-      <c r="AD67" s="2"/>
-      <c r="AE67" s="2"/>
-      <c r="AF67" s="2"/>
-      <c r="AG67" s="2"/>
-    </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-      <c r="R68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
-      <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
-      <c r="X68" s="3"/>
-      <c r="Y68" s="3"/>
-      <c r="Z68" s="3"/>
-      <c r="AA68" s="3"/>
-      <c r="AB68" s="2"/>
-      <c r="AC68" s="2"/>
-      <c r="AD68" s="2"/>
-      <c r="AE68" s="2"/>
-      <c r="AF68" s="2"/>
-      <c r="AG68" s="2"/>
-    </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P69" s="2"/>
-      <c r="Q69" s="2"/>
-      <c r="R69" s="3"/>
-      <c r="T69" s="3"/>
-      <c r="U69" s="3"/>
-      <c r="V69" s="3"/>
-      <c r="W69" s="3"/>
-      <c r="X69" s="3"/>
-      <c r="Y69" s="3"/>
-      <c r="Z69" s="3"/>
-      <c r="AA69" s="3"/>
-      <c r="AB69" s="2"/>
-      <c r="AC69" s="2"/>
-      <c r="AD69" s="2"/>
-      <c r="AE69" s="2"/>
-      <c r="AF69" s="2"/>
-      <c r="AG69" s="2"/>
-    </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-      <c r="R70" s="3"/>
-      <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
-      <c r="V70" s="3"/>
-      <c r="W70" s="3"/>
-      <c r="X70" s="3"/>
-      <c r="Y70" s="3"/>
-      <c r="Z70" s="3"/>
-      <c r="AA70" s="3"/>
-      <c r="AB70" s="2"/>
-      <c r="AC70" s="2"/>
-      <c r="AD70" s="2"/>
-      <c r="AE70" s="2"/>
-      <c r="AF70" s="2"/>
-      <c r="AG70" s="2"/>
-    </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
-      <c r="R71" s="3"/>
-      <c r="T71" s="3"/>
-      <c r="U71" s="3"/>
-      <c r="V71" s="3"/>
-      <c r="W71" s="3"/>
-      <c r="X71" s="3"/>
-      <c r="Y71" s="3"/>
-      <c r="Z71" s="3"/>
-      <c r="AA71" s="3"/>
-      <c r="AB71" s="2"/>
-      <c r="AC71" s="2"/>
-      <c r="AD71" s="2"/>
-      <c r="AE71" s="2"/>
-      <c r="AF71" s="2"/>
-      <c r="AG71" s="2"/>
-    </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P72" s="2"/>
-      <c r="Q72" s="2"/>
-      <c r="R72" s="3"/>
-      <c r="T72" s="3"/>
-      <c r="U72" s="3"/>
-      <c r="V72" s="3"/>
-      <c r="W72" s="3"/>
-      <c r="X72" s="3"/>
-      <c r="Y72" s="3"/>
-      <c r="Z72" s="3"/>
-      <c r="AA72" s="3"/>
-      <c r="AB72" s="2"/>
-      <c r="AC72" s="2"/>
-      <c r="AD72" s="2"/>
-      <c r="AE72" s="2"/>
-      <c r="AF72" s="2"/>
-      <c r="AG72" s="2"/>
-    </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P73" s="2"/>
-      <c r="Q73" s="2"/>
-      <c r="R73" s="3"/>
-      <c r="T73" s="3"/>
-      <c r="U73" s="3"/>
-      <c r="V73" s="3"/>
-      <c r="W73" s="3"/>
-      <c r="X73" s="3"/>
-      <c r="Y73" s="3"/>
-      <c r="Z73" s="3"/>
-      <c r="AA73" s="3"/>
-      <c r="AB73" s="2"/>
-      <c r="AC73" s="2"/>
-      <c r="AD73" s="2"/>
-      <c r="AE73" s="2"/>
-      <c r="AF73" s="2"/>
-      <c r="AG73" s="2"/>
-    </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P74" s="2"/>
-      <c r="Q74" s="2"/>
-      <c r="R74" s="3"/>
-      <c r="T74" s="3"/>
-      <c r="U74" s="3"/>
-      <c r="V74" s="3"/>
-      <c r="W74" s="3"/>
-      <c r="X74" s="3"/>
-      <c r="Y74" s="3"/>
-      <c r="Z74" s="3"/>
-      <c r="AA74" s="3"/>
-      <c r="AB74" s="2"/>
-      <c r="AC74" s="2"/>
-      <c r="AD74" s="2"/>
-      <c r="AE74" s="2"/>
-      <c r="AF74" s="2"/>
-      <c r="AG74" s="2"/>
-    </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P75" s="2"/>
-      <c r="Q75" s="2"/>
-      <c r="R75" s="3"/>
-      <c r="T75" s="3"/>
-      <c r="U75" s="3"/>
-      <c r="V75" s="3"/>
-      <c r="W75" s="3"/>
-      <c r="X75" s="3"/>
-      <c r="Y75" s="3"/>
-      <c r="Z75" s="3"/>
-      <c r="AA75" s="3"/>
-      <c r="AB75" s="2"/>
-      <c r="AC75" s="2"/>
-      <c r="AD75" s="2"/>
-      <c r="AE75" s="2"/>
-      <c r="AF75" s="2"/>
-      <c r="AG75" s="2"/>
-    </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
-      <c r="R76" s="3"/>
-      <c r="T76" s="3"/>
-      <c r="U76" s="3"/>
-      <c r="V76" s="3"/>
-      <c r="W76" s="3"/>
-      <c r="X76" s="3"/>
-      <c r="Y76" s="3"/>
-      <c r="Z76" s="3"/>
-      <c r="AA76" s="3"/>
-      <c r="AB76" s="2"/>
-      <c r="AC76" s="2"/>
-      <c r="AD76" s="2"/>
-      <c r="AE76" s="2"/>
-      <c r="AF76" s="2"/>
-      <c r="AG76" s="2"/>
-    </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
-      <c r="R77" s="3"/>
-      <c r="T77" s="3"/>
-      <c r="U77" s="3"/>
-      <c r="V77" s="3"/>
-      <c r="W77" s="3"/>
-      <c r="X77" s="3"/>
-      <c r="Y77" s="3"/>
-      <c r="Z77" s="3"/>
-      <c r="AA77" s="3"/>
-      <c r="AB77" s="2"/>
-      <c r="AC77" s="2"/>
-      <c r="AD77" s="2"/>
-      <c r="AE77" s="2"/>
-      <c r="AF77" s="2"/>
-      <c r="AG77" s="2"/>
-    </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P78" s="2"/>
-      <c r="Q78" s="2"/>
-      <c r="R78" s="3"/>
-      <c r="T78" s="3"/>
-      <c r="U78" s="3"/>
-      <c r="V78" s="3"/>
-      <c r="W78" s="3"/>
-      <c r="X78" s="3"/>
-      <c r="Y78" s="3"/>
-      <c r="Z78" s="3"/>
-      <c r="AA78" s="3"/>
-      <c r="AB78" s="2"/>
-      <c r="AC78" s="2"/>
-      <c r="AD78" s="2"/>
-      <c r="AE78" s="2"/>
-      <c r="AF78" s="2"/>
-      <c r="AG78" s="2"/>
-    </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P79" s="2"/>
-      <c r="Q79" s="2"/>
-      <c r="R79" s="3"/>
-      <c r="T79" s="3"/>
-      <c r="U79" s="3"/>
-      <c r="V79" s="3"/>
-      <c r="W79" s="3"/>
-      <c r="X79" s="3"/>
-      <c r="Y79" s="3"/>
-      <c r="Z79" s="3"/>
-      <c r="AA79" s="3"/>
-      <c r="AB79" s="2"/>
-      <c r="AC79" s="2"/>
-      <c r="AD79" s="2"/>
-      <c r="AE79" s="2"/>
-      <c r="AF79" s="2"/>
-      <c r="AG79" s="2"/>
-    </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P80" s="2"/>
-      <c r="Q80" s="2"/>
-      <c r="R80" s="3"/>
-      <c r="T80" s="3"/>
-      <c r="U80" s="3"/>
-      <c r="V80" s="3"/>
-      <c r="W80" s="3"/>
-      <c r="X80" s="3"/>
-      <c r="Y80" s="3"/>
-      <c r="Z80" s="3"/>
-      <c r="AA80" s="3"/>
-      <c r="AB80" s="2"/>
-      <c r="AC80" s="2"/>
-      <c r="AD80" s="2"/>
-      <c r="AE80" s="2"/>
-      <c r="AF80" s="2"/>
-      <c r="AG80" s="2"/>
-    </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P81" s="2"/>
-      <c r="Q81" s="2"/>
-      <c r="R81" s="3"/>
-      <c r="T81" s="3"/>
-      <c r="U81" s="3"/>
-      <c r="V81" s="3"/>
-      <c r="W81" s="3"/>
-      <c r="X81" s="3"/>
-      <c r="Y81" s="3"/>
-      <c r="Z81" s="3"/>
-      <c r="AA81" s="3"/>
-      <c r="AB81" s="2"/>
-      <c r="AC81" s="2"/>
-      <c r="AD81" s="2"/>
-      <c r="AE81" s="2"/>
-      <c r="AF81" s="2"/>
-      <c r="AG81" s="2"/>
-    </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P82" s="2"/>
-      <c r="Q82" s="2"/>
-      <c r="R82" s="3"/>
-      <c r="T82" s="3"/>
-      <c r="U82" s="3"/>
-      <c r="V82" s="3"/>
-      <c r="W82" s="3"/>
-      <c r="X82" s="3"/>
-      <c r="Y82" s="3"/>
-      <c r="Z82" s="3"/>
-      <c r="AA82" s="3"/>
-      <c r="AB82" s="2"/>
-      <c r="AC82" s="2"/>
-      <c r="AD82" s="2"/>
-      <c r="AE82" s="2"/>
-      <c r="AF82" s="2"/>
-      <c r="AG82" s="2"/>
-    </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P83" s="2"/>
-      <c r="Q83" s="2"/>
-      <c r="R83" s="3"/>
-      <c r="T83" s="3"/>
-      <c r="U83" s="3"/>
-      <c r="V83" s="3"/>
-      <c r="W83" s="3"/>
-      <c r="X83" s="3"/>
-      <c r="Y83" s="3"/>
-      <c r="Z83" s="3"/>
-      <c r="AA83" s="3"/>
-      <c r="AB83" s="2"/>
-      <c r="AC83" s="2"/>
-      <c r="AD83" s="2"/>
-      <c r="AE83" s="2"/>
-      <c r="AF83" s="2"/>
-      <c r="AG83" s="2"/>
-    </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P84" s="2"/>
-      <c r="Q84" s="2"/>
-      <c r="R84" s="3"/>
-      <c r="T84" s="3"/>
-      <c r="U84" s="3"/>
-      <c r="V84" s="3"/>
-      <c r="W84" s="3"/>
-      <c r="X84" s="3"/>
-      <c r="Y84" s="3"/>
-      <c r="Z84" s="3"/>
-      <c r="AA84" s="3"/>
-      <c r="AB84" s="2"/>
-      <c r="AC84" s="2"/>
-      <c r="AD84" s="2"/>
-      <c r="AE84" s="2"/>
-      <c r="AF84" s="2"/>
-      <c r="AG84" s="2"/>
-    </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P85" s="2"/>
-      <c r="Q85" s="2"/>
-      <c r="R85" s="3"/>
-      <c r="T85" s="3"/>
-      <c r="U85" s="3"/>
-      <c r="V85" s="3"/>
-      <c r="W85" s="3"/>
-      <c r="X85" s="3"/>
-      <c r="Y85" s="3"/>
-      <c r="Z85" s="3"/>
-      <c r="AA85" s="3"/>
-      <c r="AB85" s="2"/>
-      <c r="AC85" s="2"/>
-      <c r="AD85" s="2"/>
-      <c r="AE85" s="2"/>
-      <c r="AF85" s="2"/>
-      <c r="AG85" s="2"/>
-    </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="2"/>
-      <c r="R86" s="3"/>
-      <c r="T86" s="3"/>
-      <c r="U86" s="3"/>
-      <c r="V86" s="3"/>
-      <c r="W86" s="3"/>
-      <c r="X86" s="3"/>
-      <c r="Y86" s="3"/>
-      <c r="Z86" s="3"/>
-      <c r="AA86" s="3"/>
-      <c r="AB86" s="2"/>
-      <c r="AC86" s="2"/>
-      <c r="AD86" s="2"/>
-      <c r="AE86" s="2"/>
-      <c r="AF86" s="2"/>
-      <c r="AG86" s="2"/>
-    </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P87" s="2"/>
-      <c r="Q87" s="2"/>
-      <c r="R87" s="3"/>
-      <c r="T87" s="3"/>
-      <c r="U87" s="3"/>
-      <c r="V87" s="3"/>
-      <c r="W87" s="3"/>
-      <c r="X87" s="3"/>
-      <c r="Y87" s="3"/>
-      <c r="Z87" s="3"/>
-      <c r="AA87" s="3"/>
-      <c r="AB87" s="2"/>
-      <c r="AC87" s="2"/>
-      <c r="AD87" s="2"/>
-      <c r="AE87" s="2"/>
-      <c r="AF87" s="2"/>
-      <c r="AG87" s="2"/>
-    </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P88" s="2"/>
-      <c r="Q88" s="2"/>
-      <c r="R88" s="3"/>
-      <c r="T88" s="3"/>
-      <c r="U88" s="3"/>
-      <c r="V88" s="3"/>
-      <c r="W88" s="3"/>
-      <c r="X88" s="3"/>
-      <c r="Y88" s="3"/>
-      <c r="Z88" s="3"/>
-      <c r="AA88" s="3"/>
-      <c r="AB88" s="2"/>
-      <c r="AC88" s="2"/>
-      <c r="AD88" s="2"/>
-      <c r="AE88" s="2"/>
-      <c r="AF88" s="2"/>
-      <c r="AG88" s="2"/>
-    </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P89" s="2"/>
-      <c r="Q89" s="2"/>
-      <c r="R89" s="3"/>
-      <c r="T89" s="3"/>
-      <c r="U89" s="3"/>
-      <c r="V89" s="3"/>
-      <c r="W89" s="3"/>
-      <c r="X89" s="3"/>
-      <c r="Y89" s="3"/>
-      <c r="Z89" s="3"/>
-      <c r="AA89" s="3"/>
-      <c r="AB89" s="2"/>
-      <c r="AC89" s="2"/>
-      <c r="AD89" s="2"/>
-      <c r="AE89" s="2"/>
-      <c r="AF89" s="2"/>
-      <c r="AG89" s="2"/>
-    </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P90" s="2"/>
-      <c r="Q90" s="2"/>
-      <c r="R90" s="3"/>
-      <c r="T90" s="3"/>
-      <c r="U90" s="3"/>
-      <c r="V90" s="3"/>
-      <c r="W90" s="3"/>
-      <c r="X90" s="3"/>
-      <c r="Y90" s="3"/>
-      <c r="Z90" s="3"/>
-      <c r="AA90" s="3"/>
-      <c r="AB90" s="2"/>
-      <c r="AC90" s="2"/>
-      <c r="AD90" s="2"/>
-      <c r="AE90" s="2"/>
-      <c r="AF90" s="2"/>
-      <c r="AG90" s="2"/>
-    </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P91" s="2"/>
-      <c r="Q91" s="2"/>
-      <c r="R91" s="3"/>
-      <c r="T91" s="3"/>
-      <c r="U91" s="3"/>
-      <c r="V91" s="3"/>
-      <c r="W91" s="3"/>
-      <c r="X91" s="3"/>
-      <c r="Y91" s="3"/>
-      <c r="Z91" s="3"/>
-      <c r="AA91" s="3"/>
-      <c r="AB91" s="2"/>
-      <c r="AC91" s="2"/>
-      <c r="AD91" s="2"/>
-      <c r="AE91" s="2"/>
-      <c r="AF91" s="2"/>
-      <c r="AG91" s="2"/>
-    </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P92" s="2"/>
-      <c r="Q92" s="2"/>
-      <c r="R92" s="3"/>
-      <c r="T92" s="3"/>
-      <c r="U92" s="3"/>
-      <c r="V92" s="3"/>
-      <c r="W92" s="3"/>
-      <c r="X92" s="3"/>
-      <c r="Y92" s="3"/>
-      <c r="Z92" s="3"/>
-      <c r="AA92" s="3"/>
-      <c r="AB92" s="2"/>
-      <c r="AC92" s="2"/>
-      <c r="AD92" s="2"/>
-      <c r="AE92" s="2"/>
-      <c r="AF92" s="2"/>
-      <c r="AG92" s="2"/>
-    </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="2"/>
-      <c r="R93" s="3"/>
-      <c r="T93" s="3"/>
-      <c r="U93" s="3"/>
-      <c r="V93" s="3"/>
-      <c r="W93" s="3"/>
-      <c r="X93" s="3"/>
-      <c r="Y93" s="3"/>
-      <c r="Z93" s="3"/>
-      <c r="AA93" s="3"/>
-      <c r="AB93" s="2"/>
-      <c r="AC93" s="2"/>
-      <c r="AD93" s="2"/>
-      <c r="AE93" s="2"/>
-      <c r="AF93" s="2"/>
-      <c r="AG93" s="2"/>
-    </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P94" s="2"/>
-      <c r="Q94" s="2"/>
-      <c r="R94" s="3"/>
-      <c r="T94" s="3"/>
-      <c r="U94" s="3"/>
-      <c r="V94" s="3"/>
-      <c r="W94" s="3"/>
-      <c r="X94" s="3"/>
-      <c r="Y94" s="3"/>
-      <c r="Z94" s="3"/>
-      <c r="AA94" s="3"/>
-      <c r="AB94" s="2"/>
-      <c r="AC94" s="2"/>
-      <c r="AD94" s="2"/>
-      <c r="AE94" s="2"/>
-      <c r="AF94" s="2"/>
-      <c r="AG94" s="2"/>
-    </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P95" s="2"/>
-      <c r="Q95" s="2"/>
-      <c r="R95" s="3"/>
-      <c r="T95" s="3"/>
-      <c r="U95" s="3"/>
-      <c r="V95" s="3"/>
-      <c r="W95" s="3"/>
-      <c r="X95" s="3"/>
-      <c r="Y95" s="3"/>
-      <c r="Z95" s="3"/>
-      <c r="AA95" s="3"/>
-      <c r="AB95" s="2"/>
-      <c r="AC95" s="2"/>
-      <c r="AD95" s="2"/>
-      <c r="AE95" s="2"/>
-      <c r="AF95" s="2"/>
-      <c r="AG95" s="2"/>
-    </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P96" s="2"/>
-      <c r="Q96" s="2"/>
-      <c r="R96" s="3"/>
-      <c r="T96" s="3"/>
-      <c r="U96" s="3"/>
-      <c r="V96" s="3"/>
-      <c r="W96" s="3"/>
-      <c r="X96" s="3"/>
-      <c r="Y96" s="3"/>
-      <c r="Z96" s="3"/>
-      <c r="AA96" s="3"/>
-      <c r="AB96" s="2"/>
-      <c r="AC96" s="2"/>
-      <c r="AD96" s="2"/>
-      <c r="AE96" s="2"/>
-      <c r="AF96" s="2"/>
-      <c r="AG96" s="2"/>
-    </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P97" s="2"/>
-      <c r="Q97" s="2"/>
-      <c r="R97" s="3"/>
-      <c r="T97" s="3"/>
-      <c r="U97" s="3"/>
-      <c r="V97" s="3"/>
-      <c r="W97" s="3"/>
-      <c r="X97" s="3"/>
-      <c r="Y97" s="3"/>
-      <c r="Z97" s="3"/>
-      <c r="AA97" s="3"/>
-      <c r="AB97" s="2"/>
-      <c r="AC97" s="2"/>
-      <c r="AD97" s="2"/>
-      <c r="AE97" s="2"/>
-      <c r="AF97" s="2"/>
-      <c r="AG97" s="2"/>
-    </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P98" s="2"/>
-      <c r="Q98" s="2"/>
-      <c r="R98" s="3"/>
-      <c r="T98" s="3"/>
-      <c r="U98" s="3"/>
-      <c r="V98" s="3"/>
-      <c r="W98" s="3"/>
-      <c r="X98" s="3"/>
-      <c r="Y98" s="3"/>
-      <c r="Z98" s="3"/>
-      <c r="AA98" s="3"/>
-      <c r="AB98" s="2"/>
-      <c r="AC98" s="2"/>
-      <c r="AD98" s="2"/>
-      <c r="AE98" s="2"/>
-      <c r="AF98" s="2"/>
-      <c r="AG98" s="2"/>
-    </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P99" s="2"/>
-      <c r="Q99" s="2"/>
-      <c r="R99" s="3"/>
-      <c r="T99" s="3"/>
-      <c r="U99" s="3"/>
-      <c r="V99" s="3"/>
-      <c r="W99" s="3"/>
-      <c r="X99" s="3"/>
-      <c r="Y99" s="3"/>
-      <c r="Z99" s="3"/>
-      <c r="AA99" s="3"/>
-      <c r="AB99" s="2"/>
-      <c r="AC99" s="2"/>
-      <c r="AD99" s="2"/>
-      <c r="AE99" s="2"/>
-      <c r="AF99" s="2"/>
-      <c r="AG99" s="2"/>
-    </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P100" s="2"/>
-      <c r="Q100" s="2"/>
-      <c r="R100" s="3"/>
-      <c r="T100" s="3"/>
-      <c r="U100" s="3"/>
-      <c r="V100" s="3"/>
-      <c r="W100" s="3"/>
-      <c r="X100" s="3"/>
-      <c r="Y100" s="3"/>
-      <c r="Z100" s="3"/>
-      <c r="AA100" s="3"/>
-      <c r="AB100" s="2"/>
-      <c r="AC100" s="2"/>
-      <c r="AD100" s="2"/>
-      <c r="AE100" s="2"/>
-      <c r="AF100" s="2"/>
-      <c r="AG100" s="2"/>
-    </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P101" s="2"/>
-      <c r="Q101" s="2"/>
-      <c r="R101" s="3"/>
-      <c r="T101" s="3"/>
-      <c r="U101" s="3"/>
-      <c r="V101" s="3"/>
-      <c r="W101" s="3"/>
-      <c r="X101" s="3"/>
-      <c r="Y101" s="3"/>
-      <c r="Z101" s="3"/>
-      <c r="AA101" s="3"/>
-      <c r="AB101" s="2"/>
-      <c r="AC101" s="2"/>
-      <c r="AD101" s="2"/>
-      <c r="AE101" s="2"/>
-      <c r="AF101" s="2"/>
-      <c r="AG101" s="2"/>
-    </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P102" s="2"/>
-      <c r="Q102" s="2"/>
-      <c r="R102" s="3"/>
-      <c r="T102" s="3"/>
-      <c r="U102" s="3"/>
-      <c r="V102" s="3"/>
-      <c r="W102" s="3"/>
-      <c r="X102" s="3"/>
-      <c r="Y102" s="3"/>
-      <c r="Z102" s="3"/>
-      <c r="AA102" s="3"/>
-      <c r="AB102" s="2"/>
-      <c r="AC102" s="2"/>
-      <c r="AD102" s="2"/>
-      <c r="AE102" s="2"/>
-      <c r="AF102" s="2"/>
-      <c r="AG102" s="2"/>
-    </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P103" s="2"/>
-      <c r="Q103" s="2"/>
-      <c r="R103" s="3"/>
-      <c r="T103" s="3"/>
-      <c r="U103" s="3"/>
-      <c r="V103" s="3"/>
-      <c r="W103" s="3"/>
-      <c r="X103" s="3"/>
-      <c r="Y103" s="3"/>
-      <c r="Z103" s="3"/>
-      <c r="AA103" s="3"/>
-      <c r="AB103" s="2"/>
-      <c r="AC103" s="2"/>
-      <c r="AD103" s="2"/>
-      <c r="AE103" s="2"/>
-      <c r="AF103" s="2"/>
-      <c r="AG103" s="2"/>
-    </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P104" s="2"/>
-      <c r="Q104" s="2"/>
-      <c r="R104" s="3"/>
-      <c r="T104" s="3"/>
-      <c r="U104" s="3"/>
-      <c r="V104" s="3"/>
-      <c r="W104" s="3"/>
-      <c r="X104" s="3"/>
-      <c r="Y104" s="3"/>
-      <c r="Z104" s="3"/>
-      <c r="AA104" s="3"/>
-      <c r="AB104" s="2"/>
-      <c r="AC104" s="2"/>
-      <c r="AD104" s="2"/>
-      <c r="AE104" s="2"/>
-      <c r="AF104" s="2"/>
-      <c r="AG104" s="2"/>
-    </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P105" s="2"/>
-      <c r="Q105" s="2"/>
-      <c r="R105" s="3"/>
-      <c r="T105" s="3"/>
-      <c r="U105" s="3"/>
-      <c r="V105" s="3"/>
-      <c r="W105" s="3"/>
-      <c r="X105" s="3"/>
-      <c r="Y105" s="3"/>
-      <c r="Z105" s="3"/>
-      <c r="AA105" s="3"/>
-      <c r="AB105" s="2"/>
-      <c r="AC105" s="2"/>
-      <c r="AD105" s="2"/>
-      <c r="AE105" s="2"/>
-      <c r="AF105" s="2"/>
-      <c r="AG105" s="2"/>
-    </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P106" s="2"/>
-      <c r="Q106" s="2"/>
-      <c r="R106" s="3"/>
-      <c r="T106" s="3"/>
-      <c r="U106" s="3"/>
-      <c r="V106" s="3"/>
-      <c r="W106" s="3"/>
-      <c r="X106" s="3"/>
-      <c r="Y106" s="3"/>
-      <c r="Z106" s="3"/>
-      <c r="AA106" s="3"/>
-      <c r="AB106" s="2"/>
-      <c r="AC106" s="2"/>
-      <c r="AD106" s="2"/>
-      <c r="AE106" s="2"/>
-      <c r="AF106" s="2"/>
-      <c r="AG106" s="2"/>
-    </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P107" s="2"/>
-      <c r="Q107" s="2"/>
-      <c r="R107" s="3"/>
-      <c r="T107" s="3"/>
-      <c r="U107" s="3"/>
-      <c r="V107" s="3"/>
-      <c r="W107" s="3"/>
-      <c r="X107" s="3"/>
-      <c r="Y107" s="3"/>
-      <c r="Z107" s="3"/>
-      <c r="AA107" s="3"/>
-      <c r="AB107" s="2"/>
-      <c r="AC107" s="2"/>
-      <c r="AD107" s="2"/>
-      <c r="AE107" s="2"/>
-      <c r="AF107" s="2"/>
-      <c r="AG107" s="2"/>
-    </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P108" s="2"/>
-      <c r="Q108" s="2"/>
-      <c r="R108" s="3"/>
-      <c r="T108" s="3"/>
-      <c r="U108" s="3"/>
-      <c r="V108" s="3"/>
-      <c r="W108" s="3"/>
-      <c r="X108" s="3"/>
-      <c r="Y108" s="3"/>
-      <c r="Z108" s="3"/>
-      <c r="AA108" s="3"/>
-      <c r="AB108" s="2"/>
-      <c r="AC108" s="2"/>
-      <c r="AD108" s="2"/>
-      <c r="AE108" s="2"/>
-      <c r="AF108" s="2"/>
-      <c r="AG108" s="2"/>
-    </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P109" s="2"/>
-      <c r="Q109" s="2"/>
-      <c r="R109" s="3"/>
-      <c r="T109" s="3"/>
-      <c r="U109" s="3"/>
-      <c r="V109" s="3"/>
-      <c r="W109" s="3"/>
-      <c r="X109" s="3"/>
-      <c r="Y109" s="3"/>
-      <c r="Z109" s="3"/>
-      <c r="AA109" s="3"/>
-      <c r="AB109" s="2"/>
-      <c r="AC109" s="2"/>
-      <c r="AD109" s="2"/>
-      <c r="AE109" s="2"/>
-      <c r="AF109" s="2"/>
-      <c r="AG109" s="2"/>
-    </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="2"/>
-      <c r="R110" s="3"/>
-      <c r="T110" s="3"/>
-      <c r="U110" s="3"/>
-      <c r="V110" s="3"/>
-      <c r="W110" s="3"/>
-      <c r="X110" s="3"/>
-      <c r="Y110" s="3"/>
-      <c r="Z110" s="3"/>
-      <c r="AA110" s="3"/>
-      <c r="AB110" s="2"/>
-      <c r="AC110" s="2"/>
-      <c r="AD110" s="2"/>
-      <c r="AE110" s="2"/>
-      <c r="AF110" s="2"/>
-      <c r="AG110" s="2"/>
-    </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P111" s="2"/>
-      <c r="Q111" s="2"/>
-      <c r="R111" s="3"/>
-      <c r="T111" s="3"/>
-      <c r="U111" s="3"/>
-      <c r="V111" s="3"/>
-      <c r="W111" s="3"/>
-      <c r="X111" s="3"/>
-      <c r="Y111" s="3"/>
-      <c r="Z111" s="3"/>
-      <c r="AA111" s="3"/>
-      <c r="AB111" s="2"/>
-      <c r="AC111" s="2"/>
-      <c r="AD111" s="2"/>
-      <c r="AE111" s="2"/>
-      <c r="AF111" s="2"/>
-      <c r="AG111" s="2"/>
-    </row>
-    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P112" s="2"/>
-      <c r="Q112" s="2"/>
-      <c r="R112" s="3"/>
-      <c r="T112" s="3"/>
-      <c r="U112" s="3"/>
-      <c r="V112" s="3"/>
-      <c r="W112" s="3"/>
-      <c r="X112" s="3"/>
-      <c r="Y112" s="3"/>
-      <c r="Z112" s="3"/>
-      <c r="AA112" s="3"/>
-      <c r="AB112" s="2"/>
-      <c r="AC112" s="2"/>
-      <c r="AD112" s="2"/>
-      <c r="AE112" s="2"/>
-      <c r="AF112" s="2"/>
-      <c r="AG112" s="2"/>
-    </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P113" s="2"/>
-      <c r="Q113" s="2"/>
-      <c r="R113" s="3"/>
-      <c r="T113" s="3"/>
-      <c r="U113" s="3"/>
-      <c r="V113" s="3"/>
-      <c r="W113" s="3"/>
-      <c r="X113" s="3"/>
-      <c r="Y113" s="3"/>
-      <c r="Z113" s="3"/>
-      <c r="AA113" s="3"/>
-      <c r="AB113" s="2"/>
-      <c r="AC113" s="2"/>
-      <c r="AD113" s="2"/>
-      <c r="AE113" s="2"/>
-      <c r="AF113" s="2"/>
-      <c r="AG113" s="2"/>
-    </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P114" s="2"/>
-      <c r="Q114" s="2"/>
-      <c r="R114" s="3"/>
-      <c r="T114" s="3"/>
-      <c r="U114" s="3"/>
-      <c r="V114" s="3"/>
-      <c r="W114" s="3"/>
-      <c r="X114" s="3"/>
-      <c r="Y114" s="3"/>
-      <c r="Z114" s="3"/>
-      <c r="AA114" s="3"/>
-      <c r="AB114" s="2"/>
-      <c r="AC114" s="2"/>
-      <c r="AD114" s="2"/>
-      <c r="AE114" s="2"/>
-      <c r="AF114" s="2"/>
-      <c r="AG114" s="2"/>
-    </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P115" s="2"/>
-      <c r="Q115" s="2"/>
-      <c r="R115" s="3"/>
-      <c r="T115" s="3"/>
-      <c r="U115" s="3"/>
-      <c r="V115" s="3"/>
-      <c r="W115" s="3"/>
-      <c r="X115" s="3"/>
-      <c r="Y115" s="3"/>
-      <c r="Z115" s="3"/>
-      <c r="AA115" s="3"/>
-      <c r="AB115" s="2"/>
-      <c r="AC115" s="2"/>
-      <c r="AD115" s="2"/>
-      <c r="AE115" s="2"/>
-      <c r="AF115" s="2"/>
-      <c r="AG115" s="2"/>
-    </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P116" s="2"/>
-      <c r="Q116" s="2"/>
-      <c r="R116" s="3"/>
-      <c r="T116" s="3"/>
-      <c r="U116" s="3"/>
-      <c r="V116" s="3"/>
-      <c r="W116" s="3"/>
-      <c r="X116" s="3"/>
-      <c r="Y116" s="3"/>
-      <c r="Z116" s="3"/>
-      <c r="AA116" s="3"/>
-      <c r="AB116" s="2"/>
-      <c r="AC116" s="2"/>
-      <c r="AD116" s="2"/>
-      <c r="AE116" s="2"/>
-      <c r="AF116" s="2"/>
-      <c r="AG116" s="2"/>
-    </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P117" s="2"/>
-      <c r="Q117" s="2"/>
-      <c r="R117" s="3"/>
-      <c r="T117" s="3"/>
-      <c r="U117" s="3"/>
-      <c r="V117" s="3"/>
-      <c r="W117" s="3"/>
-      <c r="X117" s="3"/>
-      <c r="Y117" s="3"/>
-      <c r="Z117" s="3"/>
-      <c r="AA117" s="3"/>
-      <c r="AB117" s="2"/>
-      <c r="AC117" s="2"/>
-      <c r="AD117" s="2"/>
-      <c r="AE117" s="2"/>
-      <c r="AF117" s="2"/>
-      <c r="AG117" s="2"/>
-    </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P118" s="2"/>
-      <c r="Q118" s="2"/>
-      <c r="R118" s="3"/>
-      <c r="T118" s="3"/>
-      <c r="U118" s="3"/>
-      <c r="V118" s="3"/>
-      <c r="W118" s="3"/>
-      <c r="X118" s="3"/>
-      <c r="Y118" s="3"/>
-      <c r="Z118" s="3"/>
-      <c r="AA118" s="3"/>
-      <c r="AB118" s="2"/>
-      <c r="AC118" s="2"/>
-      <c r="AD118" s="2"/>
-      <c r="AE118" s="2"/>
-      <c r="AF118" s="2"/>
-      <c r="AG118" s="2"/>
-    </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P119" s="2"/>
-      <c r="Q119" s="2"/>
-      <c r="R119" s="3"/>
-      <c r="T119" s="3"/>
-      <c r="U119" s="3"/>
-      <c r="V119" s="3"/>
-      <c r="W119" s="3"/>
-      <c r="X119" s="3"/>
-      <c r="Y119" s="3"/>
-      <c r="Z119" s="3"/>
-      <c r="AA119" s="3"/>
-      <c r="AB119" s="2"/>
-      <c r="AC119" s="2"/>
-      <c r="AD119" s="2"/>
-      <c r="AE119" s="2"/>
-      <c r="AF119" s="2"/>
-      <c r="AG119" s="2"/>
-    </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P120" s="2"/>
-      <c r="Q120" s="2"/>
-      <c r="R120" s="3"/>
-      <c r="T120" s="3"/>
-      <c r="U120" s="3"/>
-      <c r="V120" s="3"/>
-      <c r="W120" s="3"/>
-      <c r="X120" s="3"/>
-      <c r="Y120" s="3"/>
-      <c r="Z120" s="3"/>
-      <c r="AA120" s="3"/>
-      <c r="AB120" s="2"/>
-      <c r="AC120" s="2"/>
-      <c r="AD120" s="2"/>
-      <c r="AE120" s="2"/>
-      <c r="AF120" s="2"/>
-      <c r="AG120" s="2"/>
-    </row>
-    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P121" s="2"/>
-      <c r="Q121" s="2"/>
-      <c r="R121" s="3"/>
-      <c r="T121" s="3"/>
-      <c r="U121" s="3"/>
-      <c r="V121" s="3"/>
-      <c r="W121" s="3"/>
-      <c r="X121" s="3"/>
-      <c r="Y121" s="3"/>
-      <c r="Z121" s="3"/>
-      <c r="AA121" s="3"/>
-      <c r="AB121" s="2"/>
-      <c r="AC121" s="2"/>
-      <c r="AD121" s="2"/>
-      <c r="AE121" s="2"/>
-      <c r="AF121" s="2"/>
-      <c r="AG121" s="2"/>
-    </row>
-    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P122" s="2"/>
-      <c r="Q122" s="2"/>
-      <c r="R122" s="3"/>
-      <c r="T122" s="3"/>
-      <c r="U122" s="3"/>
-      <c r="V122" s="3"/>
-      <c r="W122" s="3"/>
-      <c r="X122" s="3"/>
-      <c r="Y122" s="3"/>
-      <c r="Z122" s="3"/>
-      <c r="AA122" s="3"/>
-      <c r="AB122" s="2"/>
-      <c r="AC122" s="2"/>
-      <c r="AD122" s="2"/>
-      <c r="AE122" s="2"/>
-      <c r="AF122" s="2"/>
-      <c r="AG122" s="2"/>
-    </row>
-    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P123" s="2"/>
-      <c r="Q123" s="2"/>
-      <c r="R123" s="3"/>
-      <c r="T123" s="3"/>
-      <c r="U123" s="3"/>
-      <c r="V123" s="3"/>
-      <c r="W123" s="3"/>
-      <c r="X123" s="3"/>
-      <c r="Y123" s="3"/>
-      <c r="Z123" s="3"/>
-      <c r="AA123" s="3"/>
-      <c r="AB123" s="2"/>
-      <c r="AC123" s="2"/>
-      <c r="AD123" s="2"/>
-      <c r="AE123" s="2"/>
-      <c r="AF123" s="2"/>
-      <c r="AG123" s="2"/>
-    </row>
-    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P124" s="2"/>
-      <c r="Q124" s="2"/>
-      <c r="R124" s="3"/>
-      <c r="T124" s="3"/>
-      <c r="U124" s="3"/>
-      <c r="V124" s="3"/>
-      <c r="W124" s="3"/>
-      <c r="X124" s="3"/>
-      <c r="Y124" s="3"/>
-      <c r="Z124" s="3"/>
-      <c r="AA124" s="3"/>
-      <c r="AB124" s="2"/>
-      <c r="AC124" s="2"/>
-      <c r="AD124" s="2"/>
-      <c r="AE124" s="2"/>
-      <c r="AF124" s="2"/>
-      <c r="AG124" s="2"/>
-    </row>
-    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>1018</v>
-      </c>
-      <c r="P125" s="2"/>
-      <c r="Q125" s="2"/>
-      <c r="R125" s="3"/>
-      <c r="T125" s="3"/>
-      <c r="U125" s="3"/>
-      <c r="V125" s="3"/>
-      <c r="W125" s="3"/>
-      <c r="X125" s="3"/>
-      <c r="Y125" s="3"/>
-      <c r="Z125" s="3"/>
-      <c r="AA125" s="3"/>
-      <c r="AB125" s="2"/>
-      <c r="AC125" s="2"/>
-      <c r="AD125" s="2"/>
-      <c r="AE125" s="2"/>
-      <c r="AF125" s="2"/>
-      <c r="AG125" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>